<commit_message>
login screen,otp screen, verify screens are changed correctly
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\Lands_Time\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F93A9E6-63B3-4032-8B2E-8DF781283139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25301D29-5456-4C98-B007-DC061276E714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="292">
   <si>
     <t>key</t>
   </si>
@@ -466,6 +466,450 @@
   </si>
   <si>
     <t>మరియు</t>
+  </si>
+  <si>
+    <t>login_invalid_phone_title</t>
+  </si>
+  <si>
+    <t>Invalid Phone Number</t>
+  </si>
+  <si>
+    <t>अमान्य फ़ोन नंबर</t>
+  </si>
+  <si>
+    <t>చెల్లని ఫోన్ నంబర్</t>
+  </si>
+  <si>
+    <t>login_invalid_phone_desc</t>
+  </si>
+  <si>
+    <t>Please enter a valid 10-digit phone number</t>
+  </si>
+  <si>
+    <t>कृपया मान्य 10 अंकों का फ़ोन नंबर दर्ज करें</t>
+  </si>
+  <si>
+    <t>దయచేసి సరైన 10 అంకెల ఫోన్ నంబర్ నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>login_success_title</t>
+  </si>
+  <si>
+    <t>Login Successful! 👋</t>
+  </si>
+  <si>
+    <t>लॉगिन सफल! 👋</t>
+  </si>
+  <si>
+    <t>లాగిన్ విజయవంతం! 👋</t>
+  </si>
+  <si>
+    <t>login_success_desc</t>
+  </si>
+  <si>
+    <t>Welcome back</t>
+  </si>
+  <si>
+    <t>वापसी पर स्वागत है</t>
+  </si>
+  <si>
+    <t>మళ్లీ స్వాగతం</t>
+  </si>
+  <si>
+    <t>login_account_not_found_title</t>
+  </si>
+  <si>
+    <t>Account Not Found</t>
+  </si>
+  <si>
+    <t>खाता नहीं मिला</t>
+  </si>
+  <si>
+    <t>ఖాతా కనబడలేదు</t>
+  </si>
+  <si>
+    <t>login_account_not_found_desc</t>
+  </si>
+  <si>
+    <t>This number is not registered. Please sign up first.</t>
+  </si>
+  <si>
+    <t>यह नंबर पंजीकृत नहीं है। कृपया पहले साइन अप करें।</t>
+  </si>
+  <si>
+    <t>ఈ నంబర్ నమోదు కాలేదు. దయచేసి ముందుగా నమోదు చేసుకోండి.</t>
+  </si>
+  <si>
+    <t>login_phone_not_verified_title</t>
+  </si>
+  <si>
+    <t>फ़ोन सत्यापित नहीं है</t>
+  </si>
+  <si>
+    <t>login_phone_not_verified_desc</t>
+  </si>
+  <si>
+    <t>Please verify your phone number</t>
+  </si>
+  <si>
+    <t>कृपया अपना फ़ोन नंबर सत्यापित करें</t>
+  </si>
+  <si>
+    <t>దయచేసి మీ ఫోన్ నంబర్ ధృవీకరించండి</t>
+  </si>
+  <si>
+    <t>login_failed_title</t>
+  </si>
+  <si>
+    <t>Login Failed</t>
+  </si>
+  <si>
+    <t>लॉगिन असफल</t>
+  </si>
+  <si>
+    <t>లాగిన్ విఫలమైంది</t>
+  </si>
+  <si>
+    <t>login_network_error_title</t>
+  </si>
+  <si>
+    <t>login_network_error_desc</t>
+  </si>
+  <si>
+    <t>Failed to login. Please check your connection.</t>
+  </si>
+  <si>
+    <t>लॉगिन असफल। कृपया कनेक्शन जांचें.</t>
+  </si>
+  <si>
+    <t>లాగిన్ చేయలేకపోయాము. దయచేసి కనెక్షన్ తనిఖీ చేయండి.</t>
+  </si>
+  <si>
+    <t>login_title</t>
+  </si>
+  <si>
+    <t>Let's Sign In...</t>
+  </si>
+  <si>
+    <t>लॉगिन करें...</t>
+  </si>
+  <si>
+    <t>లాగిన్ అవ్వండి...</t>
+  </si>
+  <si>
+    <t>login_subtitle</t>
+  </si>
+  <si>
+    <t>Enter your phone number to access your account</t>
+  </si>
+  <si>
+    <t>अपने खाते तक पहुंचने के लिए अपना फोन नंबर दर्ज करें</t>
+  </si>
+  <si>
+    <t>మీ ఖాతాను ఉపయోగించడానికి మీ ఫోన్ నంబర్ నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>फोन नंबर</t>
+  </si>
+  <si>
+    <t>login_note_registered_phone</t>
+  </si>
+  <si>
+    <t>Note: Make sure you registered this phone number before signing in.</t>
+  </si>
+  <si>
+    <t>नोट: लॉगिन से पहले यह फोन नंबर पंजीकृत होना चाहिए।</t>
+  </si>
+  <si>
+    <t>గమనిక: లాగిన్ అవ్వడానికి ముందు ఈ ఫోన్ నంబర్ నమోదు చేసి ఉండాలి.</t>
+  </si>
+  <si>
+    <t>साइन इन</t>
+  </si>
+  <si>
+    <t>లాగిన్</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>रजिस्टर</t>
+  </si>
+  <si>
+    <t>already_have_account</t>
+  </si>
+  <si>
+    <t>Don't have an account?</t>
+  </si>
+  <si>
+    <t>खाता नहीं है?</t>
+  </si>
+  <si>
+    <t>ఖాతా లేదా?</t>
+  </si>
+  <si>
+    <t>otp_title_enter</t>
+  </si>
+  <si>
+    <t>Enter Verification code</t>
+  </si>
+  <si>
+    <t>सत्यापन कोड दर्ज करें</t>
+  </si>
+  <si>
+    <t>ధృవీకరణ కోడ్ నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>otp_subtitle</t>
+  </si>
+  <si>
+    <t>Please enter 4 digit verification code sent to</t>
+  </si>
+  <si>
+    <t>कृपया भेजा गया 4 अंकों का सत्यापन कोड दर्ज करें</t>
+  </si>
+  <si>
+    <t>మీకు పంపబడిన 4 అంకెల ధృవీకరణ కోడ్ నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>otp_edit</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>संपादित करें</t>
+  </si>
+  <si>
+    <t>సవరించండి</t>
+  </si>
+  <si>
+    <t>otp_timer_prefix</t>
+  </si>
+  <si>
+    <t>otp_didnt_receive</t>
+  </si>
+  <si>
+    <t>Didn't receive OTP?</t>
+  </si>
+  <si>
+    <t>OTP नहीं मिला?</t>
+  </si>
+  <si>
+    <t>OTP అందలేదా?</t>
+  </si>
+  <si>
+    <t>otp_resend</t>
+  </si>
+  <si>
+    <t>Resend Code</t>
+  </si>
+  <si>
+    <t>कोड पुनः भेजें</t>
+  </si>
+  <si>
+    <t>కోడ్ మళ్లీ పంపండి</t>
+  </si>
+  <si>
+    <t>otp_submit</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>सबमिट करें</t>
+  </si>
+  <si>
+    <t>సమర్పించండి</t>
+  </si>
+  <si>
+    <t>alert_invalid_otp_title</t>
+  </si>
+  <si>
+    <t>Invalid OTP</t>
+  </si>
+  <si>
+    <t>अमान्य OTP</t>
+  </si>
+  <si>
+    <t>చెల్లని OTP</t>
+  </si>
+  <si>
+    <t>alert_invalid_otp_desc</t>
+  </si>
+  <si>
+    <t>Please enter complete 4-digit OTP</t>
+  </si>
+  <si>
+    <t>कृपया पूरा 4 अंकों का OTP दर्ज करें</t>
+  </si>
+  <si>
+    <t>దయచేసి పూర్తి 4 అంకెల OTP నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>alert_resend_success_title</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>सफल</t>
+  </si>
+  <si>
+    <t>విజయం</t>
+  </si>
+  <si>
+    <t>alert_resend_success_desc</t>
+  </si>
+  <si>
+    <t>OTP has been resent to your phone number</t>
+  </si>
+  <si>
+    <t>OTP आपके फोन नंबर पर फिर से भेजा गया है</t>
+  </si>
+  <si>
+    <t>OTP మీ ఫోన్ నంబర్‌కు మళ్లీ పంపబడింది</t>
+  </si>
+  <si>
+    <t>alert_resend_failed_title</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>त्रुटि</t>
+  </si>
+  <si>
+    <t>లోపం</t>
+  </si>
+  <si>
+    <t>alert_resend_failed_desc</t>
+  </si>
+  <si>
+    <t>Failed to resend OTP. Please try again.</t>
+  </si>
+  <si>
+    <t>OTP पुनः भेजने में विफल। कृपया पुनः प्रयास करें।</t>
+  </si>
+  <si>
+    <t>OTP మళ్లీ పంపడంలో విఫలమైంది. దయచేసి మళ్లీ ప్రయత్నించండి.</t>
+  </si>
+  <si>
+    <t>alert_verification_failed_title</t>
+  </si>
+  <si>
+    <t>Verification Failed</t>
+  </si>
+  <si>
+    <t>सत्यापन असफल</t>
+  </si>
+  <si>
+    <t>ధృవీకరణ విఫలమైంది</t>
+  </si>
+  <si>
+    <t>alert_verification_failed_desc</t>
+  </si>
+  <si>
+    <t>Invalid OTP. Please try again.</t>
+  </si>
+  <si>
+    <t>अमान्य OTP। कृपया पुनः प्रयास करें।</t>
+  </si>
+  <si>
+    <t>చెల్లని OTP. దయచేసి మళ్లీ ప్రయత్నించండి.</t>
+  </si>
+  <si>
+    <t>alert_verify_error_title</t>
+  </si>
+  <si>
+    <t>alert_verify_error_desc</t>
+  </si>
+  <si>
+    <t>Failed to verify OTP. Please try again.</t>
+  </si>
+  <si>
+    <t>OTP सत्यापन में विफल। कृपया पुनः प्रयास करें।</t>
+  </si>
+  <si>
+    <t>OTP ధృవీకరణ విఫలమైంది. దయచేసి మళ్లీ ప్రయత్నించండి.</t>
+  </si>
+  <si>
+    <t>verify_title_prefix</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>दर्ज करें</t>
+  </si>
+  <si>
+    <t>verify_title_main</t>
+  </si>
+  <si>
+    <t>Verification code</t>
+  </si>
+  <si>
+    <t>सत्यापन कोड</t>
+  </si>
+  <si>
+    <t>ధృవీకరణ కోడ్</t>
+  </si>
+  <si>
+    <t>verify_subtitle_send_otp</t>
+  </si>
+  <si>
+    <t>We will send an OTP to your registered phone number</t>
+  </si>
+  <si>
+    <t>हम आपके पंजीकृत फ़ोन नंबर पर OTP भेजेंगे</t>
+  </si>
+  <si>
+    <t>మీ నమోదు చేసిన ఫోన్ నంబర్‌కు OTP పంపబడుతుంది</t>
+  </si>
+  <si>
+    <t>verify_label_phone</t>
+  </si>
+  <si>
+    <t>verify_button_send_otp</t>
+  </si>
+  <si>
+    <t>Send OTP</t>
+  </si>
+  <si>
+    <t>OTP भेजें</t>
+  </si>
+  <si>
+    <t>OTP పంపండి</t>
+  </si>
+  <si>
+    <t>verify_otp_send_failed_title</t>
+  </si>
+  <si>
+    <t>verify_otp_send_failed_desc</t>
+  </si>
+  <si>
+    <t>Failed to send OTP. Please try again.</t>
+  </si>
+  <si>
+    <t>OTP भेजने में विफल। कृपया पुनः प्रयास करें।</t>
+  </si>
+  <si>
+    <t>OTP పంపడంలో విఫలమైంది. దయచేసి మళ్లీ ప్రయత్నించండి.</t>
+  </si>
+  <si>
+    <t>verify_network_error_desc</t>
+  </si>
+  <si>
+    <t>Failed to send OTP. Please check your connection.</t>
+  </si>
+  <si>
+    <t>OTP भेजने में विफल। कृपया अपना कनेक्शन जांचें।</t>
+  </si>
+  <si>
+    <t>OTP పంపడంలో విఫలమైంది. దయచేసి మీ కనెక్షన్ తనిఖీ చేయండి.</t>
   </si>
 </sst>
 </file>
@@ -840,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="68" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="68" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,7 +1817,606 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="1"/>
+      <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" t="s">
+        <v>165</v>
+      </c>
+      <c r="C43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>168</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>172</v>
+      </c>
+      <c r="D45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>174</v>
+      </c>
+      <c r="B46" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>178</v>
+      </c>
+      <c r="B47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>183</v>
+      </c>
+      <c r="B49" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>187</v>
+      </c>
+      <c r="B50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" t="s">
+        <v>189</v>
+      </c>
+      <c r="D50" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" t="s">
+        <v>191</v>
+      </c>
+      <c r="C51" t="s">
+        <v>192</v>
+      </c>
+      <c r="D51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>193</v>
+      </c>
+      <c r="B52" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" t="s">
+        <v>195</v>
+      </c>
+      <c r="D52" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" t="s">
+        <v>197</v>
+      </c>
+      <c r="D53" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>199</v>
+      </c>
+      <c r="B54" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" t="s">
+        <v>200</v>
+      </c>
+      <c r="D54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>201</v>
+      </c>
+      <c r="B55" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" t="s">
+        <v>203</v>
+      </c>
+      <c r="D55" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>205</v>
+      </c>
+      <c r="B56" t="s">
+        <v>206</v>
+      </c>
+      <c r="C56" t="s">
+        <v>207</v>
+      </c>
+      <c r="D56" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>209</v>
+      </c>
+      <c r="B57" t="s">
+        <v>210</v>
+      </c>
+      <c r="C57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D57" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>213</v>
+      </c>
+      <c r="B58" t="s">
+        <v>214</v>
+      </c>
+      <c r="C58" t="s">
+        <v>215</v>
+      </c>
+      <c r="D58" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>217</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" t="s">
+        <v>219</v>
+      </c>
+      <c r="C60" t="s">
+        <v>220</v>
+      </c>
+      <c r="D60" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" t="s">
+        <v>223</v>
+      </c>
+      <c r="C61" t="s">
+        <v>224</v>
+      </c>
+      <c r="D61" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>226</v>
+      </c>
+      <c r="B62" t="s">
+        <v>227</v>
+      </c>
+      <c r="C62" t="s">
+        <v>228</v>
+      </c>
+      <c r="D62" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>230</v>
+      </c>
+      <c r="B63" t="s">
+        <v>231</v>
+      </c>
+      <c r="C63" t="s">
+        <v>232</v>
+      </c>
+      <c r="D63" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>234</v>
+      </c>
+      <c r="B64" t="s">
+        <v>235</v>
+      </c>
+      <c r="C64" t="s">
+        <v>236</v>
+      </c>
+      <c r="D64" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>238</v>
+      </c>
+      <c r="B65" t="s">
+        <v>239</v>
+      </c>
+      <c r="C65" t="s">
+        <v>240</v>
+      </c>
+      <c r="D65" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" t="s">
+        <v>243</v>
+      </c>
+      <c r="C66" t="s">
+        <v>244</v>
+      </c>
+      <c r="D66" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>246</v>
+      </c>
+      <c r="B67" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" t="s">
+        <v>248</v>
+      </c>
+      <c r="D67" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>250</v>
+      </c>
+      <c r="B68" t="s">
+        <v>251</v>
+      </c>
+      <c r="C68" t="s">
+        <v>252</v>
+      </c>
+      <c r="D68" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" t="s">
+        <v>255</v>
+      </c>
+      <c r="C69" t="s">
+        <v>256</v>
+      </c>
+      <c r="D69" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>258</v>
+      </c>
+      <c r="B70" t="s">
+        <v>259</v>
+      </c>
+      <c r="C70" t="s">
+        <v>260</v>
+      </c>
+      <c r="D70" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>262</v>
+      </c>
+      <c r="B71" t="s">
+        <v>247</v>
+      </c>
+      <c r="C71" t="s">
+        <v>248</v>
+      </c>
+      <c r="D71" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>263</v>
+      </c>
+      <c r="B72" t="s">
+        <v>264</v>
+      </c>
+      <c r="C72" t="s">
+        <v>265</v>
+      </c>
+      <c r="D72" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>267</v>
+      </c>
+      <c r="B73" t="s">
+        <v>268</v>
+      </c>
+      <c r="C73" t="s">
+        <v>269</v>
+      </c>
+      <c r="D73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>270</v>
+      </c>
+      <c r="B74" t="s">
+        <v>271</v>
+      </c>
+      <c r="C74" t="s">
+        <v>272</v>
+      </c>
+      <c r="D74" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>274</v>
+      </c>
+      <c r="B75" t="s">
+        <v>275</v>
+      </c>
+      <c r="C75" t="s">
+        <v>276</v>
+      </c>
+      <c r="D75" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>278</v>
+      </c>
+      <c r="B76" t="s">
+        <v>191</v>
+      </c>
+      <c r="C76" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B77" t="s">
+        <v>280</v>
+      </c>
+      <c r="C77" t="s">
+        <v>281</v>
+      </c>
+      <c r="D77" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>283</v>
+      </c>
+      <c r="B78" t="s">
+        <v>247</v>
+      </c>
+      <c r="C78" t="s">
+        <v>248</v>
+      </c>
+      <c r="D78" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>284</v>
+      </c>
+      <c r="B79" t="s">
+        <v>285</v>
+      </c>
+      <c r="C79" t="s">
+        <v>286</v>
+      </c>
+      <c r="D79" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>288</v>
+      </c>
+      <c r="B80" t="s">
+        <v>289</v>
+      </c>
+      <c r="C80" t="s">
+        <v>290</v>
+      </c>
+      <c r="D80" t="s">
+        <v>291</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
homescreen is fixed correctly
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\Lands_Time\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F74141-ECCB-4458-848B-BC4ACCA240AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C1F164-31AA-44D1-8B7E-782C06FE42C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="340">
   <si>
     <t>key</t>
   </si>
@@ -910,6 +910,150 @@
   </si>
   <si>
     <t>OTP పంపడంలో విఫలమైంది. దయచేసి మీ కనెక్షన్ తనిఖీ చేయండి.</t>
+  </si>
+  <si>
+    <t>home_banner_title</t>
+  </si>
+  <si>
+    <t>మీ కలల ఆస్తిని కనుగొనండి</t>
+  </si>
+  <si>
+    <t>home_banner_subtitle</t>
+  </si>
+  <si>
+    <t>Explore premium real estate options in Vizag</t>
+  </si>
+  <si>
+    <t>विजाग में प्रीमियम रियल एस्टेट विकल्पों का अन्वेषण करें</t>
+  </si>
+  <si>
+    <t>విజాగ్‌లో ప్రీమియం రియల్ ఎస్టేట్ ఎంపికలను అన్వేషించండి</t>
+  </si>
+  <si>
+    <t>home_search_placeholder</t>
+  </si>
+  <si>
+    <t>Search properties...</t>
+  </si>
+  <si>
+    <t>संपत्तियाँ खोजें...</t>
+  </si>
+  <si>
+    <t>ఆస్తులను వెతకండి...</t>
+  </si>
+  <si>
+    <t>Find Your Dream Property</t>
+  </si>
+  <si>
+    <t>अपनी सपनों की संपत्ति खोजें</t>
+  </si>
+  <si>
+    <t>home_category_sites</t>
+  </si>
+  <si>
+    <t>Sites</t>
+  </si>
+  <si>
+    <t>साइट्स</t>
+  </si>
+  <si>
+    <t>సైట్లు</t>
+  </si>
+  <si>
+    <t>home_category_sites_desc</t>
+  </si>
+  <si>
+    <t>Plot Land</t>
+  </si>
+  <si>
+    <t>प्लॉट भूमि</t>
+  </si>
+  <si>
+    <t>ప్లాట్ భూమి</t>
+  </si>
+  <si>
+    <t>home_category_resorts</t>
+  </si>
+  <si>
+    <t>Resorts</t>
+  </si>
+  <si>
+    <t>रिसॉर्ट्स</t>
+  </si>
+  <si>
+    <t>రిసార్ట్స్</t>
+  </si>
+  <si>
+    <t>home_category_resorts_desc</t>
+  </si>
+  <si>
+    <t>Luxury Getaways</t>
+  </si>
+  <si>
+    <t>लक्ज़री अवकाश स्थल</t>
+  </si>
+  <si>
+    <t>లగ్జరీ విహార ప్రదేశాలు</t>
+  </si>
+  <si>
+    <t>home_category_flats</t>
+  </si>
+  <si>
+    <t>Flats</t>
+  </si>
+  <si>
+    <t>फ्लैट्स</t>
+  </si>
+  <si>
+    <t>ఫ్లాట్స్</t>
+  </si>
+  <si>
+    <t>home_category_flats_desc</t>
+  </si>
+  <si>
+    <t>Investment Land</t>
+  </si>
+  <si>
+    <t>निवेश भूमि</t>
+  </si>
+  <si>
+    <t>పెట్టుబడి భూమి</t>
+  </si>
+  <si>
+    <t>home_category_commercial</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>व्यावसायिक</t>
+  </si>
+  <si>
+    <t>వాణిజ్య</t>
+  </si>
+  <si>
+    <t>home_category_commercial_desc</t>
+  </si>
+  <si>
+    <t>Business Spaces</t>
+  </si>
+  <si>
+    <t>व्यावसायिक स्थान</t>
+  </si>
+  <si>
+    <t>వ్యాపార స్థలాలు</t>
+  </si>
+  <si>
+    <t>home_language_modal_title</t>
+  </si>
+  <si>
+    <t>Select Your Language</t>
+  </si>
+  <si>
+    <t>अपनी भाषा चुनें</t>
+  </si>
+  <si>
+    <t>మీ భాషను ఎంచుకోండి</t>
   </si>
 </sst>
 </file>
@@ -1284,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="68" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="88" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2418,6 +2562,174 @@
         <v>291</v>
       </c>
     </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>292</v>
+      </c>
+      <c r="B81" t="s">
+        <v>302</v>
+      </c>
+      <c r="C81" t="s">
+        <v>303</v>
+      </c>
+      <c r="D81" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>294</v>
+      </c>
+      <c r="B82" t="s">
+        <v>295</v>
+      </c>
+      <c r="C82" t="s">
+        <v>296</v>
+      </c>
+      <c r="D82" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>298</v>
+      </c>
+      <c r="B83" t="s">
+        <v>299</v>
+      </c>
+      <c r="C83" t="s">
+        <v>300</v>
+      </c>
+      <c r="D83" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>304</v>
+      </c>
+      <c r="B84" t="s">
+        <v>305</v>
+      </c>
+      <c r="C84" t="s">
+        <v>306</v>
+      </c>
+      <c r="D84" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>308</v>
+      </c>
+      <c r="B85" t="s">
+        <v>309</v>
+      </c>
+      <c r="C85" t="s">
+        <v>310</v>
+      </c>
+      <c r="D85" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>312</v>
+      </c>
+      <c r="B86" t="s">
+        <v>313</v>
+      </c>
+      <c r="C86" t="s">
+        <v>314</v>
+      </c>
+      <c r="D86" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>316</v>
+      </c>
+      <c r="B87" t="s">
+        <v>317</v>
+      </c>
+      <c r="C87" t="s">
+        <v>318</v>
+      </c>
+      <c r="D87" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>320</v>
+      </c>
+      <c r="B88" t="s">
+        <v>321</v>
+      </c>
+      <c r="C88" t="s">
+        <v>322</v>
+      </c>
+      <c r="D88" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>324</v>
+      </c>
+      <c r="B89" t="s">
+        <v>325</v>
+      </c>
+      <c r="C89" t="s">
+        <v>326</v>
+      </c>
+      <c r="D89" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>328</v>
+      </c>
+      <c r="B90" t="s">
+        <v>329</v>
+      </c>
+      <c r="C90" t="s">
+        <v>330</v>
+      </c>
+      <c r="D90" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>332</v>
+      </c>
+      <c r="B91" t="s">
+        <v>333</v>
+      </c>
+      <c r="C91" t="s">
+        <v>334</v>
+      </c>
+      <c r="D91" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>336</v>
+      </c>
+      <c r="B92" t="s">
+        <v>337</v>
+      </c>
+      <c r="C92" t="s">
+        <v>338</v>
+      </c>
+      <c r="D92" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
welcome screens all are done
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\Lands_Time\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B319CB0-A69C-40AF-B13D-70E05AF855D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E364BB-515C-492A-892C-E360A536FA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1234">
   <si>
     <t>key</t>
   </si>
@@ -3640,6 +3640,102 @@
   </si>
   <si>
     <t>కట్స్</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>छोड़ें</t>
+  </si>
+  <si>
+    <t>దాటవేయి</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Find Perfect Properties</t>
+  </si>
+  <si>
+    <t>परफेक्ट प्रॉपर्टी खोजें</t>
+  </si>
+  <si>
+    <t>పరిపూర్ణ ఆస్తులను కనుగొనండి</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>आगे</t>
+  </si>
+  <si>
+    <t>తదుపరి</t>
+  </si>
+  <si>
+    <t>smart_search_label</t>
+  </si>
+  <si>
+    <t>Smart Search</t>
+  </si>
+  <si>
+    <t>स्मार्ट खोज</t>
+  </si>
+  <si>
+    <t>స్మార్ట్ శోధన</t>
+  </si>
+  <si>
+    <t>direct_property_connect_label</t>
+  </si>
+  <si>
+    <t>Direct Property Connect</t>
+  </si>
+  <si>
+    <t>प्रत्यक्ष प्रॉपर्टी कनेक्ट</t>
+  </si>
+  <si>
+    <t>ప్రత్యక్ష ప్రాపర్టీ కనెక్ట్</t>
+  </si>
+  <si>
+    <t>discover_title</t>
+  </si>
+  <si>
+    <t>Discover a place you will love to live</t>
+  </si>
+  <si>
+    <t>एक ऐसी जगह खोजें जहाँ आप रहना पसंद करेंगे</t>
+  </si>
+  <si>
+    <t>మీరు నివసించడం ఇష్టపడే స్థలాన్ని కనుగొనండి</t>
+  </si>
+  <si>
+    <t>discover_description</t>
+  </si>
+  <si>
+    <t>Browse homes for sale, original neighborhood photos, resident reviews, local insights to find what is right for you</t>
+  </si>
+  <si>
+    <t>बिक्री के लिए घर देखें, मूल पड़ोस की तस्वीरें, निवासी समीक्षाएं और स्थानीय जानकारी से अपने लिए सही जगह पाएं</t>
+  </si>
+  <si>
+    <t>అమ్మకానికి ఇళ్లను, ప్రాంతీయ ఫోటోలు, నివాసుల సమీక్షలు మరియు లోకల్ సమాచారంతో మీకు సరైన ప్రదేశాన్ని కనుగొనండి</t>
+  </si>
+  <si>
+    <t>lets_explore_button</t>
+  </si>
+  <si>
+    <t>Let's Explore</t>
+  </si>
+  <si>
+    <t>चलिए शुरू करें</t>
+  </si>
+  <si>
+    <t>చదుకుదాం / ముందుకు సాగుదాం</t>
   </si>
 </sst>
 </file>
@@ -4025,10 +4121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D391"/>
+  <dimension ref="A1:D400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" zoomScale="88" workbookViewId="0">
-      <selection activeCell="B404" sqref="B404"/>
+    <sheetView tabSelected="1" topLeftCell="A380" zoomScale="88" workbookViewId="0">
+      <selection activeCell="A403" sqref="A403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9071,6 +9167,118 @@
         <v>1201</v>
       </c>
     </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B393" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C393" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D393" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B394" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C394" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D394" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A395" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B395" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C395" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D395" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A396" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B396" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C396" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D396" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B397" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C397" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D397" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B398" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C398" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D398" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B399" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C399" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D399" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B400" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C400" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D400" t="s">
+        <v>1233</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
search screens are changed
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\Lands_Time\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E364BB-515C-492A-892C-E360A536FA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12300091-36F3-4FC0-9F24-29F48691B853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="1324">
   <si>
     <t>key</t>
   </si>
@@ -3736,6 +3736,276 @@
   </si>
   <si>
     <t>చదుకుదాం / ముందుకు సాగుదాం</t>
+  </si>
+  <si>
+    <t>settings_title</t>
+  </si>
+  <si>
+    <t>సెట్టింగ్‌లు</t>
+  </si>
+  <si>
+    <t>manage_preferences</t>
+  </si>
+  <si>
+    <t>Manage your app preferences</t>
+  </si>
+  <si>
+    <t>अपने ऐप की प्राथमिकताएँ प्रबंधित करें</t>
+  </si>
+  <si>
+    <t>మీ యాప్ అభిరుచులను నిర్వహించండి</t>
+  </si>
+  <si>
+    <t>account_title</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>खाता</t>
+  </si>
+  <si>
+    <t>ఖాతా</t>
+  </si>
+  <si>
+    <t>edit_profile</t>
+  </si>
+  <si>
+    <t>Edit Profile</t>
+  </si>
+  <si>
+    <t>प्रोफ़ाइल संपादित करें</t>
+  </si>
+  <si>
+    <t>ప్రొఫైల్ ఎడిట్ చేయండి</t>
+  </si>
+  <si>
+    <t>change_password</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>पासवर्ड बदलें</t>
+  </si>
+  <si>
+    <t>పాస్‌వర్డ్ మార్చండి</t>
+  </si>
+  <si>
+    <t>verification_status</t>
+  </si>
+  <si>
+    <t>Verification Status</t>
+  </si>
+  <si>
+    <t>सत्यापन स्थिति</t>
+  </si>
+  <si>
+    <t>తనీకరణ స్థితి</t>
+  </si>
+  <si>
+    <t>verified</t>
+  </si>
+  <si>
+    <t>తనఖీ చేయబడింది</t>
+  </si>
+  <si>
+    <t>notifications_title</t>
+  </si>
+  <si>
+    <t>सूचनाएँ</t>
+  </si>
+  <si>
+    <t>property_alerts</t>
+  </si>
+  <si>
+    <t>Property Alerts</t>
+  </si>
+  <si>
+    <t>प्रॉपर्टी अलर्ट</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ అలర్ట్స్</t>
+  </si>
+  <si>
+    <t>price_changes</t>
+  </si>
+  <si>
+    <t>Price Changes</t>
+  </si>
+  <si>
+    <t>कीमत में बदलाव</t>
+  </si>
+  <si>
+    <t>ధర మార్పులు</t>
+  </si>
+  <si>
+    <t>messages</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>संदेश</t>
+  </si>
+  <si>
+    <t>సందేశాలు</t>
+  </si>
+  <si>
+    <t>marketing_emails</t>
+  </si>
+  <si>
+    <t>Marketing Emails</t>
+  </si>
+  <si>
+    <t>मार्केटिंग ईमेल</t>
+  </si>
+  <si>
+    <t>మార్కెటింగ్ ఇమెయిల్స్</t>
+  </si>
+  <si>
+    <t>privacy_title</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>गोपनीयता</t>
+  </si>
+  <si>
+    <t>గోప్యత</t>
+  </si>
+  <si>
+    <t>profile_visible</t>
+  </si>
+  <si>
+    <t>Profile Visible</t>
+  </si>
+  <si>
+    <t>प्रोफ़ाइल दिखाई दे</t>
+  </si>
+  <si>
+    <t>ప్రొఫైల్ కనిపించాలి</t>
+  </si>
+  <si>
+    <t>show_activity</t>
+  </si>
+  <si>
+    <t>Show Activity</t>
+  </si>
+  <si>
+    <t>गतिविधि दिखाएँ</t>
+  </si>
+  <si>
+    <t>కార్యకలాపం చూపించండి</t>
+  </si>
+  <si>
+    <t>allow_messages</t>
+  </si>
+  <si>
+    <t>Allow Messages</t>
+  </si>
+  <si>
+    <t>संदेशों की अनुमति दें</t>
+  </si>
+  <si>
+    <t>సందేశాలను అనుమతించండి</t>
+  </si>
+  <si>
+    <t>general_title</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>सामान्य</t>
+  </si>
+  <si>
+    <t>సాధారణ</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>भाषा</t>
+  </si>
+  <si>
+    <t>భాష</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>मुद्रा</t>
+  </si>
+  <si>
+    <t>కరెన్సీ</t>
+  </si>
+  <si>
+    <t>help_support</t>
+  </si>
+  <si>
+    <t>Help &amp; Support</t>
+  </si>
+  <si>
+    <t>सहायता और समर्थन</t>
+  </si>
+  <si>
+    <t>సహాయం &amp; మద్దతు</t>
+  </si>
+  <si>
+    <t>selectDistrict.title</t>
+  </si>
+  <si>
+    <t>Select District in Andhra</t>
+  </si>
+  <si>
+    <t>आंध्र में जिला चुनें</t>
+  </si>
+  <si>
+    <t>ఆంధ్రప్రదేశ్ జిల్లాను ఎంచుకోండి</t>
+  </si>
+  <si>
+    <t>selectDistrict.searchPlaceholder</t>
+  </si>
+  <si>
+    <t>Search districts in Andhra...</t>
+  </si>
+  <si>
+    <t>आंध्र के जिलों को खोजें...</t>
+  </si>
+  <si>
+    <t>ఆంధ్రా జిల్లాలను శోధించండి...</t>
+  </si>
+  <si>
+    <t>selectDistrict.noResults</t>
+  </si>
+  <si>
+    <t>No districts found for "{query}"</t>
+  </si>
+  <si>
+    <t>{query} के लिए कोई जिला नहीं मिला</t>
+  </si>
+  <si>
+    <t>{query} కి సంబంధించిన జిల్లాలు లభించలేదు</t>
+  </si>
+  <si>
+    <t>selectDistrict.propertiesAvailable</t>
+  </si>
+  <si>
+    <t>properties available</t>
+  </si>
+  <si>
+    <t>प्रॉपर्टीज उपलब्ध</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీలు అందుబాటులో ఉన్నాయి</t>
   </si>
 </sst>
 </file>
@@ -4121,10 +4391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D400"/>
+  <dimension ref="A1:D431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" zoomScale="88" workbookViewId="0">
-      <selection activeCell="A403" sqref="A403"/>
+    <sheetView tabSelected="1" topLeftCell="A416" zoomScale="88" workbookViewId="0">
+      <selection activeCell="A435" sqref="A435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9279,6 +9549,342 @@
         <v>1233</v>
       </c>
     </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B403" t="s">
+        <v>378</v>
+      </c>
+      <c r="C403" t="s">
+        <v>379</v>
+      </c>
+      <c r="D403" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B404" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C404" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D404" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B406" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C406" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D406" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A407" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B407" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C407" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D407" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A408" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B408" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C408" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D408" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A409" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B409" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C409" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D409" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A410" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B410" t="s">
+        <v>37</v>
+      </c>
+      <c r="C410" t="s">
+        <v>38</v>
+      </c>
+      <c r="D410" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B412" t="s">
+        <v>374</v>
+      </c>
+      <c r="C412" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D412" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B413" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C413" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D413" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B414" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C414" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D414" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B415" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C415" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D415" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B416" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C416" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D416" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B418" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C418" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D418" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B419" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C419" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D419" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B420" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C420" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D420" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B421" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C421" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D421" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B423" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C423" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D423" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B424" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C424" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D424" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B425" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C425" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D425" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B426" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C426" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D426" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B428" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C428" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D428" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B429" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C429" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D429" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B430" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C430" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D430" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B431" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C431" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D431" t="s">
+        <v>1323</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
for ther commercial property fetch frontend fixed and username stored in 3 languages in backend
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\Lands_Time\Landstime_Androidapp\Frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\LandsTime-301-12-2025\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12300091-36F3-4FC0-9F24-29F48691B853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74111343-B98C-41CA-906F-3209E43F1AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="1324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="1416">
   <si>
     <t>key</t>
   </si>
@@ -3966,24 +3966,12 @@
     <t>Select District in Andhra</t>
   </si>
   <si>
-    <t>आंध्र में जिला चुनें</t>
-  </si>
-  <si>
-    <t>ఆంధ్రప్రదేశ్ జిల్లాను ఎంచుకోండి</t>
-  </si>
-  <si>
     <t>selectDistrict.searchPlaceholder</t>
   </si>
   <si>
     <t>Search districts in Andhra...</t>
   </si>
   <si>
-    <t>आंध्र के जिलों को खोजें...</t>
-  </si>
-  <si>
-    <t>ఆంధ్రా జిల్లాలను శోధించండి...</t>
-  </si>
-  <si>
     <t>selectDistrict.noResults</t>
   </si>
   <si>
@@ -3993,19 +3981,307 @@
     <t>{query} के लिए कोई जिला नहीं मिला</t>
   </si>
   <si>
-    <t>{query} కి సంబంధించిన జిల్లాలు లభించలేదు</t>
-  </si>
-  <si>
     <t>selectDistrict.propertiesAvailable</t>
   </si>
   <si>
     <t>properties available</t>
   </si>
   <si>
-    <t>प्रॉपर्टीज उपलब्ध</t>
-  </si>
-  <si>
-    <t>ప్రాపర్టీలు అందుబాటులో ఉన్నాయి</t>
+    <t>आंध्र प्रदेश में जिला चुनें</t>
+  </si>
+  <si>
+    <t>ఆంధ్రప్రదేశ్‌లో జిల్లాను ఎంచుకోండి</t>
+  </si>
+  <si>
+    <t>आंध्र प्रदेश में जिलों को खोजें...</t>
+  </si>
+  <si>
+    <t>ఆంధ్రప్రదేశ్‌లో జిల్లాలను శోధించండి...</t>
+  </si>
+  <si>
+    <t>{query} కోసం జిల్లాలు కనుగొనబడలేదు</t>
+  </si>
+  <si>
+    <t>संपत्तियां उपलब्ध हैं</t>
+  </si>
+  <si>
+    <t>ఆస్తులు అందుబాటులో ఉన్నాయి</t>
+  </si>
+  <si>
+    <t>districts.anantapur</t>
+  </si>
+  <si>
+    <t>Anantapur</t>
+  </si>
+  <si>
+    <t>अनंतपुर</t>
+  </si>
+  <si>
+    <t>అనంతపురం</t>
+  </si>
+  <si>
+    <t>districts.chittoor</t>
+  </si>
+  <si>
+    <t>Chittoor</t>
+  </si>
+  <si>
+    <t>चित्तूर</t>
+  </si>
+  <si>
+    <t>చిత్తూరు</t>
+  </si>
+  <si>
+    <t>districts.eastgodavari</t>
+  </si>
+  <si>
+    <t>East Godavari</t>
+  </si>
+  <si>
+    <t>पूर्वी गोदावरी</t>
+  </si>
+  <si>
+    <t>తూర్పు గోదావరి</t>
+  </si>
+  <si>
+    <t>districts.guntur</t>
+  </si>
+  <si>
+    <t>Guntur</t>
+  </si>
+  <si>
+    <t>गुंटूर</t>
+  </si>
+  <si>
+    <t>గుంటూరు</t>
+  </si>
+  <si>
+    <t>districts.kadapa</t>
+  </si>
+  <si>
+    <t>Kadapa</t>
+  </si>
+  <si>
+    <t>कडपा</t>
+  </si>
+  <si>
+    <t>కడప</t>
+  </si>
+  <si>
+    <t>districts.krishna</t>
+  </si>
+  <si>
+    <t>Krishna</t>
+  </si>
+  <si>
+    <t>कृष्णा</t>
+  </si>
+  <si>
+    <t>కృష్ణా</t>
+  </si>
+  <si>
+    <t>districts.kurnool</t>
+  </si>
+  <si>
+    <t>Kurnool</t>
+  </si>
+  <si>
+    <t>कर्नूल</t>
+  </si>
+  <si>
+    <t>కర్నూలు</t>
+  </si>
+  <si>
+    <t>districts.nellore</t>
+  </si>
+  <si>
+    <t>Nellore</t>
+  </si>
+  <si>
+    <t>नेल्लोर</t>
+  </si>
+  <si>
+    <t>నెల్లూరు</t>
+  </si>
+  <si>
+    <t>districts.srikakulam</t>
+  </si>
+  <si>
+    <t>Srikakulam</t>
+  </si>
+  <si>
+    <t>श्रीकाकुलम</t>
+  </si>
+  <si>
+    <t>శ్రీకాకుళం</t>
+  </si>
+  <si>
+    <t>districts.visakhapatnam</t>
+  </si>
+  <si>
+    <t>Visakhapatnam</t>
+  </si>
+  <si>
+    <t>विशाखापत्तनम</t>
+  </si>
+  <si>
+    <t>విశాఖపట్టణం</t>
+  </si>
+  <si>
+    <t>districts.vizianagaram</t>
+  </si>
+  <si>
+    <t>Vizianagaram</t>
+  </si>
+  <si>
+    <t>विजयनगरम</t>
+  </si>
+  <si>
+    <t>విజయనగరం</t>
+  </si>
+  <si>
+    <t>districts.westgodavari</t>
+  </si>
+  <si>
+    <t>West Godavari</t>
+  </si>
+  <si>
+    <t>पश्चिम गोदावरी</t>
+  </si>
+  <si>
+    <t>పశ్చిమ గోదావరి</t>
+  </si>
+  <si>
+    <t>areas.akkayapalem</t>
+  </si>
+  <si>
+    <t>Akkayapalem</t>
+  </si>
+  <si>
+    <t>अक्कायापलेम</t>
+  </si>
+  <si>
+    <t>అక్కయ్యపాలెం</t>
+  </si>
+  <si>
+    <t>areas.anandapuram</t>
+  </si>
+  <si>
+    <t>Anandapuram</t>
+  </si>
+  <si>
+    <t>आनंदपुरम</t>
+  </si>
+  <si>
+    <t>ఆనందపురం</t>
+  </si>
+  <si>
+    <t>areas.boyapalem</t>
+  </si>
+  <si>
+    <t>Boyapalem</t>
+  </si>
+  <si>
+    <t>बोयापलेम</t>
+  </si>
+  <si>
+    <t>బోయపాలెం</t>
+  </si>
+  <si>
+    <t>areas.chinnagadili</t>
+  </si>
+  <si>
+    <t>Chinna Gadili</t>
+  </si>
+  <si>
+    <t>चिन्ना गडिली</t>
+  </si>
+  <si>
+    <t>చిన్న గడిలి</t>
+  </si>
+  <si>
+    <t>areas.dwarkanagar</t>
+  </si>
+  <si>
+    <t>Dwarka Nagar</t>
+  </si>
+  <si>
+    <t>द्वारका नगर</t>
+  </si>
+  <si>
+    <t>ద్వారకా నగర్</t>
+  </si>
+  <si>
+    <t>areas.gajuwaka</t>
+  </si>
+  <si>
+    <t>Gajuwaka</t>
+  </si>
+  <si>
+    <t>गाजुवाका</t>
+  </si>
+  <si>
+    <t>గాజువాక</t>
+  </si>
+  <si>
+    <t>areas.kommadi</t>
+  </si>
+  <si>
+    <t>Kommadi</t>
+  </si>
+  <si>
+    <t>कोम्मडी</t>
+  </si>
+  <si>
+    <t>కొమ్మడి</t>
+  </si>
+  <si>
+    <t>selectSite.title</t>
+  </si>
+  <si>
+    <t>Select Resort</t>
+  </si>
+  <si>
+    <t>रिसॉर्ट चुनें</t>
+  </si>
+  <si>
+    <t>రిసార్ట్‌ను ఎంచుకోండి</t>
+  </si>
+  <si>
+    <t>selectSite.searchPlaceholder</t>
+  </si>
+  <si>
+    <t>Search properties in</t>
+  </si>
+  <si>
+    <t>में संपत्तियों को खोजें</t>
+  </si>
+  <si>
+    <t>లో ఆస్తులను శోధించండి</t>
+  </si>
+  <si>
+    <t>selectSite.noResults</t>
+  </si>
+  <si>
+    <t>No properties found</t>
+  </si>
+  <si>
+    <t>कोई संपत्ति नहीं मिली</t>
+  </si>
+  <si>
+    <t>ఆస్తులు కనుగొనబడలేదు</t>
+  </si>
+  <si>
+    <t>sidebar_menu_my_properties</t>
+  </si>
+  <si>
+    <t>My Properties</t>
+  </si>
+  <si>
+    <t>मेरी प्रॉपर्टीज़</t>
+  </si>
+  <si>
+    <t>నా ఆస్తులు</t>
   </si>
 </sst>
 </file>
@@ -4391,10 +4667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D431"/>
+  <dimension ref="A1:D459"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" zoomScale="88" workbookViewId="0">
-      <selection activeCell="A435" sqref="A435"/>
+    <sheetView tabSelected="1" topLeftCell="C447" zoomScale="88" workbookViewId="0">
+      <selection activeCell="J465" sqref="J465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9829,60 +10105,382 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A428" t="s">
-        <v>1308</v>
-      </c>
-      <c r="B428" t="s">
-        <v>1309</v>
-      </c>
-      <c r="C428" t="s">
-        <v>1310</v>
-      </c>
-      <c r="D428" t="s">
-        <v>1311</v>
-      </c>
-    </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="B429" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="C429" t="s">
-        <v>1314</v>
+        <v>1317</v>
       </c>
       <c r="D429" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="B430" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="C430" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D430" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
-        <v>1320</v>
+        <v>1312</v>
       </c>
       <c r="B431" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C431" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D431" t="s">
         <v>1321</v>
       </c>
-      <c r="C431" t="s">
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B432" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C432" t="s">
         <v>1322</v>
       </c>
-      <c r="D431" t="s">
+      <c r="D432" t="s">
         <v>1323</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B434" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C434" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D434" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B435" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C435" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D435" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B436" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C436" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D436" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B437" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C437" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D437" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A438" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B438" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C438" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D438" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A439" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B439" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C439" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D439" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A440" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B440" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C440" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D440" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A441" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B441" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C441" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D441" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A442" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B442" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C442" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D442" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A443" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B443" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C443" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D443" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A444" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B444" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C444" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D444" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B445" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C445" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D445" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B447" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C447" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D447" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B448" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C448" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D448" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B449" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C449" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D449" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B450" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C450" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D450" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B451" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C451" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D451" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B452" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C452" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D452" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B453" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C453" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D453" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B455" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C455" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D455" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B456" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C456" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D456" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B457" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C457" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D457" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B459" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C459" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D459" t="s">
+        <v>1415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
industry is working good
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\LandsTime-301-12-2025\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEEB34F-2820-4B47-888A-A8E0010FA8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA4BD3B-589D-40C2-9AD4-1591FEC39E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3767" uniqueCount="2998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4079" uniqueCount="3143">
   <si>
     <t>key</t>
   </si>
@@ -9050,6 +9050,441 @@
   </si>
   <si>
     <t>మీరు మీ ఫోటో లైబ్రరీకి యాక్సెస్ మంజూరు చేయాలి.</t>
+  </si>
+  <si>
+    <t>industry_location</t>
+  </si>
+  <si>
+    <t>industry_area_required</t>
+  </si>
+  <si>
+    <t>industry_neighborhood</t>
+  </si>
+  <si>
+    <t>industry_enter_location</t>
+  </si>
+  <si>
+    <t>industry_enter_area</t>
+  </si>
+  <si>
+    <t>industry_add_room_details</t>
+  </si>
+  <si>
+    <t>industry_no_of_washrooms</t>
+  </si>
+  <si>
+    <t>industry_washroom_none</t>
+  </si>
+  <si>
+    <t>industry_washroom_shared</t>
+  </si>
+  <si>
+    <t>industry_add_area_details</t>
+  </si>
+  <si>
+    <t>industry_availability_status</t>
+  </si>
+  <si>
+    <t>industry_ready_to_move</t>
+  </si>
+  <si>
+    <t>industry_under_construction</t>
+  </si>
+  <si>
+    <t>industry_age_of_property</t>
+  </si>
+  <si>
+    <t>industry_age_0_1</t>
+  </si>
+  <si>
+    <t>industry_age_1_5</t>
+  </si>
+  <si>
+    <t>industry_age_5_10</t>
+  </si>
+  <si>
+    <t>industry_age_10plus</t>
+  </si>
+  <si>
+    <t>industry_possession_by</t>
+  </si>
+  <si>
+    <t>industry_expected_by</t>
+  </si>
+  <si>
+    <t>industry_possession_immediate</t>
+  </si>
+  <si>
+    <t>industry_possession_3months</t>
+  </si>
+  <si>
+    <t>industry_possession_6months</t>
+  </si>
+  <si>
+    <t>industry_possession_2026</t>
+  </si>
+  <si>
+    <t>industry_possession_2027</t>
+  </si>
+  <si>
+    <t>industry_possession_2028</t>
+  </si>
+  <si>
+    <t>industry_possession_2029</t>
+  </si>
+  <si>
+    <t>industry_possession_2030</t>
+  </si>
+  <si>
+    <t>industry_ownership</t>
+  </si>
+  <si>
+    <t>industry_ownership_freehold</t>
+  </si>
+  <si>
+    <t>industry_ownership_leasehold</t>
+  </si>
+  <si>
+    <t>industry_ownership_company</t>
+  </si>
+  <si>
+    <t>industry_ownership_other</t>
+  </si>
+  <si>
+    <t>industry_approved_by</t>
+  </si>
+  <si>
+    <t>industry_approved_authority</t>
+  </si>
+  <si>
+    <t>industry_approved_industry_type</t>
+  </si>
+  <si>
+    <t>industry_select_industry</t>
+  </si>
+  <si>
+    <t>industry_expected_price</t>
+  </si>
+  <si>
+    <t>industry_enter_price</t>
+  </si>
+  <si>
+    <t>industry_dg_ups_included</t>
+  </si>
+  <si>
+    <t>industry_price_negotiable</t>
+  </si>
+  <si>
+    <t>industry_tax_excluded</t>
+  </si>
+  <si>
+    <t>industry_pre_leased</t>
+  </si>
+  <si>
+    <t>industry_yes</t>
+  </si>
+  <si>
+    <t>industry_no</t>
+  </si>
+  <si>
+    <t>industry_current_rent</t>
+  </si>
+  <si>
+    <t>industry_lease_tenure</t>
+  </si>
+  <si>
+    <t>industry_description</t>
+  </si>
+  <si>
+    <t>industry_describe_placeholder</t>
+  </si>
+  <si>
+    <t>industry_amenities</t>
+  </si>
+  <si>
+    <t>industry_other_features</t>
+  </si>
+  <si>
+    <t>industry_wheelchair_friendly</t>
+  </si>
+  <si>
+    <t>industry_location_advantages</t>
+  </si>
+  <si>
+    <t>industry_price_required</t>
+  </si>
+  <si>
+    <t>industry_description_required</t>
+  </si>
+  <si>
+    <t>industry_details_saved</t>
+  </si>
+  <si>
+    <t>industry_moving_next</t>
+  </si>
+  <si>
+    <t>పొరుగు ప్రాంతం</t>
+  </si>
+  <si>
+    <t>స్థానాన్ని నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>ప్రాంతాన్ని నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>తరలించడానికి సిద్ధంగా ఉంది</t>
+  </si>
+  <si>
+    <t>స్వాధీనం ద్వారా</t>
+  </si>
+  <si>
+    <t>ఆశించిన ద్వారా</t>
+  </si>
+  <si>
+    <t>తక్షణ</t>
+  </si>
+  <si>
+    <t>ద్వారా ఆమోదించబడింది</t>
+  </si>
+  <si>
+    <t>ఆశించిన ధర</t>
+  </si>
+  <si>
+    <t>ధరను నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>ధర చర్చించదగినది</t>
+  </si>
+  <si>
+    <t>ముందుగా లీజుకు ఇవ్వబడింది</t>
+  </si>
+  <si>
+    <t>లీజు వ్యవధి సంవత్సరాలలో</t>
+  </si>
+  <si>
+    <t>మీ ఆస్తిని ప్రత్యేకంగా చేసేది ఏమిటో వ్రాయండి</t>
+  </si>
+  <si>
+    <t>వీల్‌చైర్ స్నేహపూర్వకం</t>
+  </si>
+  <si>
+    <t>తదుపరికి వెళ్తోంది</t>
+  </si>
+  <si>
+    <t>क्षेत्र आवश्यक</t>
+  </si>
+  <si>
+    <t>पड़ोस/इलाका</t>
+  </si>
+  <si>
+    <t>स्थान दर्ज करें</t>
+  </si>
+  <si>
+    <t>क्षेत्र दर्ज करें</t>
+  </si>
+  <si>
+    <t>कमरे का विवरण जोड़ें</t>
+  </si>
+  <si>
+    <t>क्षेत्र विवरण जोड़ें</t>
+  </si>
+  <si>
+    <t>स्थानांतरण के लिए तैयार</t>
+  </si>
+  <si>
+    <t>कब्ज़ा द्वारा</t>
+  </si>
+  <si>
+    <t>अपेक्षित द्वारा</t>
+  </si>
+  <si>
+    <t>कंपनी स्वामित्व</t>
+  </si>
+  <si>
+    <t>द्वारा स्वीकृत</t>
+  </si>
+  <si>
+    <t>उद्योग प्रकार के लिए स्वीकृत</t>
+  </si>
+  <si>
+    <t>अपेक्षित मूल्य</t>
+  </si>
+  <si>
+    <t>मूल्य दर्ज करें</t>
+  </si>
+  <si>
+    <t>कर और सरकारी शुल्क बाहर</t>
+  </si>
+  <si>
+    <t>पूर्व-पट्टे पर दिया गया</t>
+  </si>
+  <si>
+    <t>पट्टा अवधि वर्षों में</t>
+  </si>
+  <si>
+    <t>लिखें कि आपकी संपत्ति को क्या अद्वितीय बनाता है</t>
+  </si>
+  <si>
+    <t>स्थान लाभ</t>
+  </si>
+  <si>
+    <t>मूल्य आवश्यक</t>
+  </si>
+  <si>
+    <t>विवरण आवश्यक</t>
+  </si>
+  <si>
+    <t>आगे बढ़ रहे हैं</t>
+  </si>
+  <si>
+    <t>No of Wash Rooms</t>
+  </si>
+  <si>
+    <t>Moving to Next</t>
+  </si>
+  <si>
+    <t>industry_unit_sqft</t>
+  </si>
+  <si>
+    <t>industry_unit_sqm</t>
+  </si>
+  <si>
+    <t>industry_unit_acre</t>
+  </si>
+  <si>
+    <t>industry_plot_building_facing</t>
+  </si>
+  <si>
+    <t>Industrial Plot/Building Facing</t>
+  </si>
+  <si>
+    <t>औद्योगिक भूखंड/भवन का सामना</t>
+  </si>
+  <si>
+    <t>పారిశ్రామిక ప్లాట్/భవనం ముఖం</t>
+  </si>
+  <si>
+    <t>industry_entrance_direction</t>
+  </si>
+  <si>
+    <t>Main Entrance/Gate Direction</t>
+  </si>
+  <si>
+    <t>industry_machinery_direction</t>
+  </si>
+  <si>
+    <t>Heavy Machinery Placement Direction</t>
+  </si>
+  <si>
+    <t>भारी मशीनरी स्थापना दिशा</t>
+  </si>
+  <si>
+    <t>భారీ యంత్రాల స్థాన దిశ</t>
+  </si>
+  <si>
+    <t>industry_production_direction</t>
+  </si>
+  <si>
+    <t>Production/Manufacturing Area Direction</t>
+  </si>
+  <si>
+    <t>उत्पादन/विनिर्माण क्षेत्र दिशा</t>
+  </si>
+  <si>
+    <t>ఉత్పత్తి/తయారీ ప్రాంత దిశ</t>
+  </si>
+  <si>
+    <t>industry_raw_material_direction</t>
+  </si>
+  <si>
+    <t>Raw Material Storage Direction</t>
+  </si>
+  <si>
+    <t>कच्चे माल भंडारण दिशा</t>
+  </si>
+  <si>
+    <t>ముడి పదార్థాల నిల్వ దిశ</t>
+  </si>
+  <si>
+    <t>industry_finished_goods_direction</t>
+  </si>
+  <si>
+    <t>Finished Goods Storage Direction</t>
+  </si>
+  <si>
+    <t>तैयार माल भंडारण दिशा</t>
+  </si>
+  <si>
+    <t>పూర్తి వస్తువుల నిల్వ దిశ</t>
+  </si>
+  <si>
+    <t>industry_office_direction</t>
+  </si>
+  <si>
+    <t>Office/Administration Area Direction</t>
+  </si>
+  <si>
+    <t>कार्यालय/प्रशासन क्षेत्र दिशा</t>
+  </si>
+  <si>
+    <t>కార్యాలయ/పరిపాలన ప్రాంత దిశ</t>
+  </si>
+  <si>
+    <t>industry_electrical_direction</t>
+  </si>
+  <si>
+    <t>Electrical/Generator/Boiler Area Direction</t>
+  </si>
+  <si>
+    <t>विद्युत/जनरेटर/बॉयलर क्षेत्र दिशा</t>
+  </si>
+  <si>
+    <t>విద్యుత్/జనరేటర్/బాయిలర్ ప్రాంత దిశ</t>
+  </si>
+  <si>
+    <t>industry_water_direction</t>
+  </si>
+  <si>
+    <t>Water Source/Tank Direction</t>
+  </si>
+  <si>
+    <t>जल स्रोत/टैंक दिशा</t>
+  </si>
+  <si>
+    <t>నీటి మూలం/ట్యాంక్ దిశ</t>
+  </si>
+  <si>
+    <t>industry_waste_direction</t>
+  </si>
+  <si>
+    <t>Waste/Scrap Area Direction</t>
+  </si>
+  <si>
+    <t>अपशिष्ट/स्क्रैप क्षेत्र दिशा</t>
+  </si>
+  <si>
+    <t>వ్యర్థ/స్క్రాప్ ప్రాంత దిశ</t>
+  </si>
+  <si>
+    <t>industry_washroom_direction</t>
+  </si>
+  <si>
+    <t>शौचालय दिशा</t>
+  </si>
+  <si>
+    <t>వాష్‌రూమ్‌ల దిశ</t>
+  </si>
+  <si>
+    <t>vaastu_option_towards_south</t>
+  </si>
+  <si>
+    <t>vaastu_option_towards_west</t>
+  </si>
+  <si>
+    <t>ఉత్తరం నీటి వనరు</t>
+  </si>
+  <si>
+    <t>सभी दिशाओं में समान ऊंचाई</t>
   </si>
 </sst>
 </file>
@@ -9435,10 +9870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D1043"/>
+  <dimension ref="A1:D1123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1039" zoomScale="73" workbookViewId="0">
-      <selection activeCell="D1059" sqref="D1059"/>
+    <sheetView tabSelected="1" topLeftCell="A1096" zoomScale="69" workbookViewId="0">
+      <selection activeCell="B1133" sqref="B1133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23046,6 +23481,1098 @@
         <v>2997</v>
       </c>
     </row>
+    <row r="1045" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1045" t="s">
+        <v>2998</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D1045" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1046" t="s">
+        <v>2999</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>2454</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>3071</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1047" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>3072</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>3055</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1048" t="s">
+        <v>3001</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>3073</v>
+      </c>
+      <c r="D1048" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1049" t="s">
+        <v>3002</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>3074</v>
+      </c>
+      <c r="D1049" t="s">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1050" t="s">
+        <v>3003</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>2460</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>3075</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1051" t="s">
+        <v>3004</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>3093</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>2473</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1052" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>2476</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>2477</v>
+      </c>
+      <c r="D1052" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1053" t="s">
+        <v>3006</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>2480</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>2481</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1054" t="s">
+        <v>3007</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>2525</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>3076</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1055" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1056" t="s">
+        <v>3009</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>2545</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>3077</v>
+      </c>
+      <c r="D1056" t="s">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1057" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D1057" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1058" t="s">
+        <v>3011</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>2550</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D1058" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1059" t="s">
+        <v>3012</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1060" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>1754</v>
+      </c>
+      <c r="D1060" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1061" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D1061" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1062" t="s">
+        <v>3015</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>1762</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1063" t="s">
+        <v>3016</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>3078</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1064" t="s">
+        <v>3017</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>3079</v>
+      </c>
+      <c r="D1064" t="s">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1065" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>3061</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1066" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>2565</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1067" t="s">
+        <v>3020</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>2567</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1068" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>2573</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>2574</v>
+      </c>
+      <c r="D1068" t="s">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1069" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>2577</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>2578</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1070" t="s">
+        <v>3023</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>2582</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>2583</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1071" t="s">
+        <v>3024</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C1071" t="s">
+        <v>2586</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1072" t="s">
+        <v>3025</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>2589</v>
+      </c>
+      <c r="C1072" t="s">
+        <v>2590</v>
+      </c>
+      <c r="D1072" t="s">
+        <v>2591</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1073" t="s">
+        <v>3026</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C1073" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D1073" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1074" t="s">
+        <v>3027</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C1074" t="s">
+        <v>1766</v>
+      </c>
+      <c r="D1074" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1075" t="s">
+        <v>3028</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D1075" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1076" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>2652</v>
+      </c>
+      <c r="C1076" t="s">
+        <v>3080</v>
+      </c>
+      <c r="D1076" t="s">
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1077" t="s">
+        <v>3030</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>2507</v>
+      </c>
+      <c r="C1077" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D1077" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1078" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>2657</v>
+      </c>
+      <c r="C1078" t="s">
+        <v>3081</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>3062</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1079" t="s">
+        <v>3032</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>2661</v>
+      </c>
+      <c r="C1079" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D1079" t="s">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1080" t="s">
+        <v>3033</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>2665</v>
+      </c>
+      <c r="C1080" t="s">
+        <v>3082</v>
+      </c>
+      <c r="D1080" t="s">
+        <v>2667</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1081" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>2669</v>
+      </c>
+      <c r="C1081" t="s">
+        <v>2670</v>
+      </c>
+      <c r="D1081" t="s">
+        <v>2671</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1082" t="s">
+        <v>3035</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>2673</v>
+      </c>
+      <c r="C1082" t="s">
+        <v>3083</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>3063</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1083" t="s">
+        <v>3036</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C1083" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>3064</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1084" t="s">
+        <v>3037</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>2683</v>
+      </c>
+      <c r="C1084" t="s">
+        <v>2684</v>
+      </c>
+      <c r="D1084" t="s">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1085" t="s">
+        <v>3038</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C1085" t="s">
+        <v>2687</v>
+      </c>
+      <c r="D1085" t="s">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1086" t="s">
+        <v>3039</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>3085</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>2691</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1087" t="s">
+        <v>3040</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>2694</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>3086</v>
+      </c>
+      <c r="D1087" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1088" t="s">
+        <v>3041</v>
+      </c>
+      <c r="B1088" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1088" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1088" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1089" t="s">
+        <v>3042</v>
+      </c>
+      <c r="B1089" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1089" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1089" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1090" t="s">
+        <v>3043</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>2700</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>2701</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1091" t="s">
+        <v>3044</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>2704</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>3087</v>
+      </c>
+      <c r="D1091" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1092" t="s">
+        <v>3045</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C1092" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D1092" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1093" t="s">
+        <v>3046</v>
+      </c>
+      <c r="B1093" t="s">
+        <v>2711</v>
+      </c>
+      <c r="C1093" t="s">
+        <v>3088</v>
+      </c>
+      <c r="D1093" t="s">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1094" t="s">
+        <v>3047</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>2715</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>2716</v>
+      </c>
+      <c r="D1094" t="s">
+        <v>2717</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1095" t="s">
+        <v>3048</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>2724</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>2725</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>2726</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1096" t="s">
+        <v>3049</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>2728</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>2729</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1097" t="s">
+        <v>3050</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>3089</v>
+      </c>
+      <c r="D1097" t="s">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1098" t="s">
+        <v>3051</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>2677</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>3090</v>
+      </c>
+      <c r="D1098" t="s">
+        <v>2679</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1099" t="s">
+        <v>3052</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>2709</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>3091</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1100" t="s">
+        <v>3053</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>2804</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>2805</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>2806</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1101" t="s">
+        <v>3054</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>3094</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>3092</v>
+      </c>
+      <c r="D1101" t="s">
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1103" t="s">
+        <v>3095</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>2530</v>
+      </c>
+      <c r="D1103" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1104" t="s">
+        <v>3096</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>2534</v>
+      </c>
+      <c r="D1104" t="s">
+        <v>2534</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1105" t="s">
+        <v>3097</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>2538</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>2539</v>
+      </c>
+      <c r="D1105" t="s">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1106" t="s">
+        <v>3098</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>3099</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>3100</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1107" t="s">
+        <v>3102</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>3103</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>2159</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1108" t="s">
+        <v>3104</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>3105</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>3106</v>
+      </c>
+      <c r="D1108" t="s">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1109" t="s">
+        <v>3108</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>3109</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D1109" t="s">
+        <v>3111</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1110" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>3113</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>3114</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>3115</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1111" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>3117</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>3118</v>
+      </c>
+      <c r="D1111" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1112" t="s">
+        <v>3120</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>3121</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>3122</v>
+      </c>
+      <c r="D1112" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1113" t="s">
+        <v>3124</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>3125</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>3126</v>
+      </c>
+      <c r="D1113" t="s">
+        <v>3127</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1114" t="s">
+        <v>3128</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>3129</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>3130</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1115" t="s">
+        <v>3132</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>3134</v>
+      </c>
+      <c r="D1115" t="s">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1116" t="s">
+        <v>3136</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>2397</v>
+      </c>
+      <c r="C1116" t="s">
+        <v>3137</v>
+      </c>
+      <c r="D1116" t="s">
+        <v>3138</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1117" t="s">
+        <v>3139</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>2198</v>
+      </c>
+      <c r="C1117" t="s">
+        <v>2199</v>
+      </c>
+      <c r="D1117" t="s">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1118" t="s">
+        <v>3140</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>2206</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>2207</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1119" t="s">
+        <v>2414</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>2214</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>2215</v>
+      </c>
+      <c r="D1119" t="s">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1120" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>2234</v>
+      </c>
+      <c r="C1120" t="s">
+        <v>2235</v>
+      </c>
+      <c r="D1120" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1121" t="s">
+        <v>2419</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>2254</v>
+      </c>
+      <c r="C1121" t="s">
+        <v>2255</v>
+      </c>
+      <c r="D1121" t="s">
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1122" t="s">
+        <v>2420</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>2274</v>
+      </c>
+      <c r="C1122" t="s">
+        <v>3142</v>
+      </c>
+      <c r="D1122" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1123" t="s">
+        <v>2418</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>2290</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>2291</v>
+      </c>
+      <c r="D1123" t="s">
+        <v>2292</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
plot is working good and correct
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d8c1b1ae6504acc/Desktop/Technoji/LandsTime-301-12-2025/Landstime_Androidapp/Frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{2BA4BD3B-589D-40C2-9AD4-1591FEC39E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE252E0B-77FA-4681-8A13-44354F6706B6}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{767929E8-DE60-4946-918E-ACB6D13E7776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EF2D477-F9C2-437F-8D56-F22C71816D7E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5007" uniqueCount="3773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5153" uniqueCount="3856">
   <si>
     <t>key</t>
   </si>
@@ -11110,9 +11110,6 @@
     <t>plot_amenity_parking</t>
   </si>
   <si>
-    <t>plot_location_advantages</t>
-  </si>
-  <si>
     <t>plot_location_metro</t>
   </si>
   <si>
@@ -11375,6 +11372,258 @@
   </si>
   <si>
     <t>పారిశ్రామిక భూమి</t>
+  </si>
+  <si>
+    <t>hospitality_amenity_water_storage</t>
+  </si>
+  <si>
+    <t>hospitality_amenity_air_conditioned</t>
+  </si>
+  <si>
+    <t>hospitality_amenity_vaastu_complex</t>
+  </si>
+  <si>
+    <t>hospitality_amenity_fire_alarm</t>
+  </si>
+  <si>
+    <t>hospitality_amenity_visitor_parking</t>
+  </si>
+  <si>
+    <t>hospitality_loc_metro_station</t>
+  </si>
+  <si>
+    <t>hospitality_loc_railway_station</t>
+  </si>
+  <si>
+    <t>plot_amenity_water_storage</t>
+  </si>
+  <si>
+    <t>plot_amenity_vaastu_complex</t>
+  </si>
+  <si>
+    <t>plot_amenity_visitor_parking</t>
+  </si>
+  <si>
+    <t>plot_loc_metro_station</t>
+  </si>
+  <si>
+    <t>plot_loc_school</t>
+  </si>
+  <si>
+    <t>plot_loc_hospital</t>
+  </si>
+  <si>
+    <t>plot_loc_market</t>
+  </si>
+  <si>
+    <t>plot_loc_railway_station</t>
+  </si>
+  <si>
+    <t>plot_loc_airport</t>
+  </si>
+  <si>
+    <t>plot_loc_mall</t>
+  </si>
+  <si>
+    <t>plot_loc_highway</t>
+  </si>
+  <si>
+    <t>'+Water Storage</t>
+  </si>
+  <si>
+    <t>'+पानी की भंडारण सुविधा</t>
+  </si>
+  <si>
+    <t>'+నీటి నిల్వ</t>
+  </si>
+  <si>
+    <t>'+currently Air Conditioned</t>
+  </si>
+  <si>
+    <t>'+वर्तमान में वातानुकूलित</t>
+  </si>
+  <si>
+    <t>'+ప్రస్తుతం వాతానుకూలత</t>
+  </si>
+  <si>
+    <t>'+Vaastu Complex</t>
+  </si>
+  <si>
+    <t>'+वास्तु कॉम्प्लेक्स</t>
+  </si>
+  <si>
+    <t>'+వాస్తు కాంప్లెక్స్</t>
+  </si>
+  <si>
+    <t>'+Security fire Alarm</t>
+  </si>
+  <si>
+    <t>'+सुरक्षा अग्नि अलार्म</t>
+  </si>
+  <si>
+    <t>'+భద్రత అగ్ని అలారం</t>
+  </si>
+  <si>
+    <t>'+Visitor Parking</t>
+  </si>
+  <si>
+    <t>'+आगंतुकों के लिए पार्किंग</t>
+  </si>
+  <si>
+    <t>'+సందర్శకుల పార్కింగ్</t>
+  </si>
+  <si>
+    <t>'+Close to Metro Station</t>
+  </si>
+  <si>
+    <t>'+मेट्रो स्टेशन के पास</t>
+  </si>
+  <si>
+    <t>'+మెట్రో స్టేషన్ దగ్గర</t>
+  </si>
+  <si>
+    <t>'+Close to School</t>
+  </si>
+  <si>
+    <t>'+स्कूल के पास</t>
+  </si>
+  <si>
+    <t>'+పాఠశాల దగ్గర</t>
+  </si>
+  <si>
+    <t>'+Close to Hospital</t>
+  </si>
+  <si>
+    <t>'+अस्पताल के पास</t>
+  </si>
+  <si>
+    <t>'+ఆసుపత్రి దగ్గర</t>
+  </si>
+  <si>
+    <t>'+Close to Market</t>
+  </si>
+  <si>
+    <t>'+मार्केट के पास</t>
+  </si>
+  <si>
+    <t>'+మార్కెట్ దగ్గర</t>
+  </si>
+  <si>
+    <t>'+Close to Railway Station</t>
+  </si>
+  <si>
+    <t>'+रेलवे स्टेशन के पास</t>
+  </si>
+  <si>
+    <t>'+రైల्वే స్టేషన్ దగ్గర</t>
+  </si>
+  <si>
+    <t>'+Close to Airport</t>
+  </si>
+  <si>
+    <t>'+हवाई अड्डे के पास</t>
+  </si>
+  <si>
+    <t>'+విమానాశ్రయం దగ్గర</t>
+  </si>
+  <si>
+    <t>'+Close to Mall</t>
+  </si>
+  <si>
+    <t>'+मॉल के पास</t>
+  </si>
+  <si>
+    <t>'+మాల్ దగ్గర</t>
+  </si>
+  <si>
+    <t>'+Close to Highway</t>
+  </si>
+  <si>
+    <t>'+हाईवे के पास</t>
+  </si>
+  <si>
+    <t>'+హైవే దగ్గర</t>
+  </si>
+  <si>
+    <t>'+రైల్వే స్టేషన్ దగ్గర</t>
+  </si>
+  <si>
+    <t>'+ Shed</t>
+  </si>
+  <si>
+    <t>'+शेड</t>
+  </si>
+  <si>
+    <t>'+షెడ్</t>
+  </si>
+  <si>
+    <t>'+ Room(s)</t>
+  </si>
+  <si>
+    <t>'+कमरा(ए)</t>
+  </si>
+  <si>
+    <t>'+గది(లు)</t>
+  </si>
+  <si>
+    <t>'+ Washroom</t>
+  </si>
+  <si>
+    <t>'+शौचालय</t>
+  </si>
+  <si>
+    <t>'+వాష్‌రూమ్</t>
+  </si>
+  <si>
+    <t>'+ Other</t>
+  </si>
+  <si>
+    <t>'+अन्य</t>
+  </si>
+  <si>
+    <t>'+ఇతర</t>
+  </si>
+  <si>
+    <t>'+ Water Storage</t>
+  </si>
+  <si>
+    <t>'+ Vaastu Complex</t>
+  </si>
+  <si>
+    <t>'+ Visitor Parking</t>
+  </si>
+  <si>
+    <t>'+ Close to Metro Station</t>
+  </si>
+  <si>
+    <t>'+ Close to School</t>
+  </si>
+  <si>
+    <t>'+ Close to Hospital</t>
+  </si>
+  <si>
+    <t>'+ Close to Market</t>
+  </si>
+  <si>
+    <t>'+ Close to Railway Station</t>
+  </si>
+  <si>
+    <t>'+ Close to Airport</t>
+  </si>
+  <si>
+    <t>'+ Close to Mall</t>
+  </si>
+  <si>
+    <t>'+ Close to Highway</t>
+  </si>
+  <si>
+    <t>'+ More Pricing Details</t>
+  </si>
+  <si>
+    <t>'+अधिक मूल्य विवरण</t>
+  </si>
+  <si>
+    <t>'+మరిన్ని ధర వివరాలు</t>
   </si>
 </sst>
 </file>
@@ -11760,10 +12009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D1378"/>
+  <dimension ref="A1:D1408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1237" zoomScale="69" workbookViewId="0">
-      <selection activeCell="A1264" sqref="A1264"/>
+    <sheetView tabSelected="1" topLeftCell="A1294" zoomScale="69" workbookViewId="0">
+      <selection activeCell="D1322" sqref="D1322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28743,68 +28992,56 @@
       <c r="A1289" t="s">
         <v>3621</v>
       </c>
-      <c r="B1289" t="e" cm="1">
-        <f t="array" ref="B1289">+ Shed</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1289" t="e" cm="1">
-        <f t="array" ref="C1289">+ शेड</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1289" t="e" cm="1">
-        <f t="array" ref="D1289">+ షెడ్</f>
-        <v>#NAME?</v>
+      <c r="B1289" t="s">
+        <v>3830</v>
+      </c>
+      <c r="C1289" t="s">
+        <v>3831</v>
+      </c>
+      <c r="D1289" t="s">
+        <v>3832</v>
       </c>
     </row>
     <row r="1290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1290" t="s">
         <v>3622</v>
       </c>
-      <c r="B1290" t="e" cm="1">
-        <f t="array" aca="1" ref="B1290" ca="1">+ Room(s)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1290" t="e" cm="1">
-        <f t="array" ref="C1290">+ कमरा/कमरे</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1290" t="e" cm="1">
-        <f t="array" ref="D1290">+ గది/గదులు</f>
-        <v>#NAME?</v>
+      <c r="B1290" t="s">
+        <v>3833</v>
+      </c>
+      <c r="C1290" t="s">
+        <v>3834</v>
+      </c>
+      <c r="D1290" t="s">
+        <v>3835</v>
       </c>
     </row>
     <row r="1291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1291" t="s">
         <v>3623</v>
       </c>
-      <c r="B1291" t="e" cm="1">
-        <f t="array" ref="B1291">+ Washroom</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1291" t="e" cm="1">
-        <f t="array" ref="C1291">+ शौचालय</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1291" t="e" cm="1">
-        <f t="array" ref="D1291">+ వాష్‌రూమ్</f>
-        <v>#NAME?</v>
+      <c r="B1291" t="s">
+        <v>3836</v>
+      </c>
+      <c r="C1291" t="s">
+        <v>3837</v>
+      </c>
+      <c r="D1291" t="s">
+        <v>3838</v>
       </c>
     </row>
     <row r="1292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1292" t="s">
         <v>3624</v>
       </c>
-      <c r="B1292" t="e" cm="1">
-        <f t="array" ref="B1292">+ Other</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1292" t="e" cm="1">
-        <f t="array" ref="C1292">+ अन्य</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1292" t="e" cm="1">
-        <f t="array" ref="D1292">+ ఇతర</f>
-        <v>#NAME?</v>
+      <c r="B1292" t="s">
+        <v>3839</v>
+      </c>
+      <c r="C1292" t="s">
+        <v>3840</v>
+      </c>
+      <c r="D1292" t="s">
+        <v>3841</v>
       </c>
     </row>
     <row r="1294" spans="1:4" x14ac:dyDescent="0.3">
@@ -29007,17 +29244,14 @@
       <c r="A1308" t="s">
         <v>3652</v>
       </c>
-      <c r="B1308" t="e" cm="1">
-        <f t="array" ref="B1308">+ Add more pricing details</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1308" t="e" cm="1">
-        <f t="array" ref="C1308">+ अधिक मूल्य विवरण जोड़ें</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1308" t="e" cm="1">
-        <f t="array" ref="D1308">+ మరిన్ని ధర వివరాలు జోడించండి</f>
-        <v>#NAME?</v>
+      <c r="B1308" t="s">
+        <v>3853</v>
+      </c>
+      <c r="C1308" t="s">
+        <v>3854</v>
+      </c>
+      <c r="D1308" t="s">
+        <v>3855</v>
       </c>
     </row>
     <row r="1309" spans="1:4" x14ac:dyDescent="0.3">
@@ -29160,89 +29394,46 @@
         <v>2717</v>
       </c>
     </row>
-    <row r="1319" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1319" t="s">
-        <v>3679</v>
-      </c>
-      <c r="B1319" t="e" cm="1">
-        <f t="array" ref="B1319">+Water Storage</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1319" t="e" cm="1">
-        <f t="array" ref="C1319">+जल भंडारण</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1319" t="e" cm="1">
-        <f t="array" ref="D1319">+నీటి నిల్వ</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
     <row r="1320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1320" t="s">
-        <v>3680</v>
-      </c>
-      <c r="B1320" t="e" cm="1">
-        <f t="array" ref="B1320">+currently Air Conditioned</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1320" t="e" cm="1">
-        <f t="array" ref="C1320">+वर्तमान में वातानुकूलित</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1320" t="e" cm="1">
-        <f t="array" ref="D1320">+ప్రస్తుతం ఏసీ ఉంది</f>
-        <v>#NAME?</v>
+        <v>3679</v>
+      </c>
+      <c r="B1320" t="s">
+        <v>3842</v>
+      </c>
+      <c r="C1320" t="s">
+        <v>3791</v>
+      </c>
+      <c r="D1320" t="s">
+        <v>3792</v>
       </c>
     </row>
     <row r="1321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1321" t="s">
         <v>3681</v>
       </c>
-      <c r="B1321" t="e" cm="1">
-        <f t="array" ref="B1321">+Vaastu Complex</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1321" t="e" cm="1">
-        <f t="array" ref="C1321">+वास्तु कॉम्प्लेक्स</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1321" t="e" cm="1">
-        <f t="array" ref="D1321">+వాస్తు సముదాయం</f>
-        <v>#NAME?</v>
+      <c r="B1321" t="s">
+        <v>3843</v>
+      </c>
+      <c r="C1321" t="s">
+        <v>3797</v>
+      </c>
+      <c r="D1321" t="s">
+        <v>3798</v>
       </c>
     </row>
     <row r="1322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1322" t="s">
-        <v>3682</v>
-      </c>
-      <c r="B1322" t="e" cm="1">
-        <f t="array" ref="B1322">+Security fire Alarm</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1322" t="e" cm="1">
-        <f t="array" ref="C1322">+फायर अलार्म सुरक्षा</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1322" t="e" cm="1">
-        <f t="array" ref="D1322">+ఫైర్ అలారం భద్రత</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="1323" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1323" t="s">
         <v>3683</v>
       </c>
-      <c r="B1323" t="e" cm="1">
-        <f t="array" ref="B1323">+Visitor Parking</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1323" t="e" cm="1">
-        <f t="array" ref="C1323">+आगंतुक पार्किंग</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1323" t="e" cm="1">
-        <f t="array" ref="D1323">+సందర్శకుల పార్కింగ్</f>
-        <v>#NAME?</v>
+      <c r="B1322" t="s">
+        <v>3844</v>
+      </c>
+      <c r="C1322" t="s">
+        <v>3803</v>
+      </c>
+      <c r="D1322" t="s">
+        <v>3804</v>
       </c>
     </row>
     <row r="1324" spans="1:4" x14ac:dyDescent="0.3">
@@ -29250,157 +29441,119 @@
         <v>3684</v>
       </c>
       <c r="B1324" t="s">
-        <v>1734</v>
+        <v>3845</v>
       </c>
       <c r="C1324" t="s">
-        <v>1735</v>
+        <v>3806</v>
       </c>
       <c r="D1324" t="s">
-        <v>1736</v>
+        <v>3807</v>
       </c>
     </row>
     <row r="1325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1325" t="s">
         <v>3685</v>
       </c>
-      <c r="B1325" t="e" cm="1">
-        <f t="array" ref="B1325">+Close to Metro Station</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1325" t="e" cm="1">
-        <f t="array" ref="C1325">+मेट्रो स्टेशन के पास</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1325" t="e" cm="1">
-        <f t="array" ref="D1325">+మెట్రో స్టేషన్ దగ్గర</f>
-        <v>#NAME?</v>
+      <c r="B1325" t="s">
+        <v>3846</v>
+      </c>
+      <c r="C1325" t="s">
+        <v>3809</v>
+      </c>
+      <c r="D1325" t="s">
+        <v>3810</v>
       </c>
     </row>
     <row r="1326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1326" t="s">
         <v>3686</v>
       </c>
-      <c r="B1326" t="e" cm="1">
-        <f t="array" ref="B1326">+Close to School</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1326" t="e" cm="1">
-        <f t="array" ref="C1326">+स्कूल के पास</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1326" t="e" cm="1">
-        <f t="array" ref="D1326">+పాఠశాల దగ్గర</f>
-        <v>#NAME?</v>
+      <c r="B1326" t="s">
+        <v>3847</v>
+      </c>
+      <c r="C1326" t="s">
+        <v>3812</v>
+      </c>
+      <c r="D1326" t="s">
+        <v>3813</v>
       </c>
     </row>
     <row r="1327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1327" t="s">
         <v>3687</v>
       </c>
-      <c r="B1327" t="e" cm="1">
-        <f t="array" ref="B1327">+Close to Hospital</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1327" t="e" cm="1">
-        <f t="array" ref="C1327">+अस्पताल के पास</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1327" t="e" cm="1">
-        <f t="array" ref="D1327">+ఆసుపత్రి దగ్గర</f>
-        <v>#NAME?</v>
+      <c r="B1327" t="s">
+        <v>3848</v>
+      </c>
+      <c r="C1327" t="s">
+        <v>3815</v>
+      </c>
+      <c r="D1327" t="s">
+        <v>3816</v>
       </c>
     </row>
     <row r="1328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1328" t="s">
         <v>3688</v>
       </c>
-      <c r="B1328" t="e" cm="1">
-        <f t="array" ref="B1328">+Close to Market</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1328" t="e" cm="1">
-        <f t="array" ref="C1328">+बाजार के पास</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1328" t="e" cm="1">
-        <f t="array" ref="D1328">+మార్కెట్ దగ్గర</f>
-        <v>#NAME?</v>
+      <c r="B1328" t="s">
+        <v>3849</v>
+      </c>
+      <c r="C1328" t="s">
+        <v>3818</v>
+      </c>
+      <c r="D1328" t="s">
+        <v>3829</v>
       </c>
     </row>
     <row r="1329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1329" t="s">
         <v>3689</v>
       </c>
-      <c r="B1329" t="e" cm="1">
-        <f t="array" ref="B1329">+Close to Railway Station</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1329" t="e" cm="1">
-        <f t="array" ref="C1329">+रेलवे स्टेशन के पास</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1329" t="e" cm="1">
-        <f t="array" ref="D1329">+రైల్వే స్టేషన్ దగ్గర</f>
-        <v>#NAME?</v>
+      <c r="B1329" t="s">
+        <v>3850</v>
+      </c>
+      <c r="C1329" t="s">
+        <v>3821</v>
+      </c>
+      <c r="D1329" t="s">
+        <v>3822</v>
       </c>
     </row>
     <row r="1330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1330" t="s">
         <v>3690</v>
       </c>
-      <c r="B1330" t="e" cm="1">
-        <f t="array" ref="B1330">+Close to Airport</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1330" t="e" cm="1">
-        <f t="array" ref="C1330">+हवाई अड्डे के पास</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1330" t="e" cm="1">
-        <f t="array" ref="D1330">+విమానాశ్రయం దగ్గర</f>
-        <v>#NAME?</v>
+      <c r="B1330" t="s">
+        <v>3851</v>
+      </c>
+      <c r="C1330" t="s">
+        <v>3824</v>
+      </c>
+      <c r="D1330" t="s">
+        <v>3825</v>
       </c>
     </row>
     <row r="1331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1331" t="s">
         <v>3691</v>
       </c>
-      <c r="B1331" t="e" cm="1">
-        <f t="array" ref="B1331">+Close to Mall</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1331" t="e" cm="1">
-        <f t="array" ref="C1331">+मॉल के पास</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1331" t="e" cm="1">
-        <f t="array" ref="D1331">+మాల్ దగ్గర</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="1332" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1332" t="s">
-        <v>3692</v>
-      </c>
-      <c r="B1332" t="e" cm="1">
-        <f t="array" ref="B1332">+Close to Highway</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C1332" t="e" cm="1">
-        <f t="array" ref="C1332">+राजमार्ग के पास</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D1332" t="e" cm="1">
-        <f t="array" ref="D1332">+హైవే దగ్గర</f>
-        <v>#NAME?</v>
+      <c r="B1331" t="s">
+        <v>3852</v>
+      </c>
+      <c r="C1331" t="s">
+        <v>3827</v>
+      </c>
+      <c r="D1331" t="s">
+        <v>3828</v>
       </c>
     </row>
     <row r="1334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1334" t="s">
+        <v>3692</v>
+      </c>
+      <c r="B1334" t="s">
         <v>3693</v>
-      </c>
-      <c r="B1334" t="s">
-        <v>3694</v>
       </c>
       <c r="C1334" t="s">
         <v>1538</v>
@@ -29411,24 +29564,24 @@
     </row>
     <row r="1335" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1335" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="B1335" t="s">
         <v>2154</v>
       </c>
       <c r="C1335" t="s">
+        <v>3695</v>
+      </c>
+      <c r="D1335" t="s">
         <v>3696</v>
-      </c>
-      <c r="D1335" t="s">
-        <v>3697</v>
       </c>
     </row>
     <row r="1336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1336" t="s">
+        <v>3697</v>
+      </c>
+      <c r="B1336" t="s">
         <v>3698</v>
-      </c>
-      <c r="B1336" t="s">
-        <v>3699</v>
       </c>
       <c r="C1336" t="s">
         <v>2359</v>
@@ -29439,35 +29592,35 @@
     </row>
     <row r="1337" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1337" t="s">
-        <v>3700</v>
+        <v>3699</v>
       </c>
       <c r="B1337" t="s">
         <v>2162</v>
       </c>
       <c r="C1337" t="s">
+        <v>3700</v>
+      </c>
+      <c r="D1337" t="s">
         <v>3701</v>
-      </c>
-      <c r="D1337" t="s">
-        <v>3702</v>
       </c>
     </row>
     <row r="1338" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1338" t="s">
-        <v>3703</v>
+        <v>3702</v>
       </c>
       <c r="B1338" t="s">
         <v>2166</v>
       </c>
       <c r="C1338" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D1338" t="s">
         <v>3704</v>
-      </c>
-      <c r="D1338" t="s">
-        <v>3705</v>
       </c>
     </row>
     <row r="1339" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1339" t="s">
-        <v>3706</v>
+        <v>3705</v>
       </c>
       <c r="B1339" t="s">
         <v>2170</v>
@@ -29481,7 +29634,7 @@
     </row>
     <row r="1340" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1340" t="s">
-        <v>3707</v>
+        <v>3706</v>
       </c>
       <c r="B1340" t="s">
         <v>2174</v>
@@ -29490,12 +29643,12 @@
         <v>2175</v>
       </c>
       <c r="D1340" t="s">
-        <v>3708</v>
+        <v>3707</v>
       </c>
     </row>
     <row r="1341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1341" t="s">
-        <v>3709</v>
+        <v>3708</v>
       </c>
       <c r="B1341" t="s">
         <v>2178</v>
@@ -29504,12 +29657,12 @@
         <v>2179</v>
       </c>
       <c r="D1341" t="s">
-        <v>3710</v>
+        <v>3709</v>
       </c>
     </row>
     <row r="1342" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1342" t="s">
-        <v>3711</v>
+        <v>3710</v>
       </c>
       <c r="B1342" t="s">
         <v>2182</v>
@@ -29518,12 +29671,12 @@
         <v>2183</v>
       </c>
       <c r="D1342" t="s">
-        <v>3712</v>
+        <v>3711</v>
       </c>
     </row>
     <row r="1343" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1343" t="s">
-        <v>3713</v>
+        <v>3712</v>
       </c>
       <c r="B1343" t="s">
         <v>2186</v>
@@ -29537,16 +29690,16 @@
     </row>
     <row r="1344" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1344" t="s">
-        <v>3714</v>
+        <v>3713</v>
       </c>
       <c r="B1344" t="s">
         <v>2190</v>
       </c>
       <c r="C1344" t="s">
+        <v>3714</v>
+      </c>
+      <c r="D1344" t="s">
         <v>3715</v>
-      </c>
-      <c r="D1344" t="s">
-        <v>3716</v>
       </c>
     </row>
     <row r="1346" spans="1:4" x14ac:dyDescent="0.3">
@@ -29677,7 +29830,7 @@
     </row>
     <row r="1355" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1355" t="s">
-        <v>3717</v>
+        <v>3716</v>
       </c>
       <c r="B1355" t="s">
         <v>2202</v>
@@ -29700,21 +29853,21 @@
         <v>2215</v>
       </c>
       <c r="D1356" t="s">
-        <v>3718</v>
+        <v>3717</v>
       </c>
     </row>
     <row r="1357" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1357" t="s">
+        <v>3718</v>
+      </c>
+      <c r="B1357" t="s">
         <v>3719</v>
       </c>
-      <c r="B1357" t="s">
+      <c r="C1357" t="s">
         <v>3720</v>
       </c>
-      <c r="C1357" t="s">
+      <c r="D1357" t="s">
         <v>3721</v>
-      </c>
-      <c r="D1357" t="s">
-        <v>3722</v>
       </c>
     </row>
     <row r="1358" spans="1:4" x14ac:dyDescent="0.3">
@@ -29725,7 +29878,7 @@
         <v>2234</v>
       </c>
       <c r="C1358" t="s">
-        <v>3723</v>
+        <v>3722</v>
       </c>
       <c r="D1358" t="s">
         <v>2236</v>
@@ -29733,16 +29886,16 @@
     </row>
     <row r="1359" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1359" t="s">
-        <v>3724</v>
+        <v>3723</v>
       </c>
       <c r="B1359" t="s">
         <v>2238</v>
       </c>
       <c r="C1359" t="s">
+        <v>3724</v>
+      </c>
+      <c r="D1359" t="s">
         <v>3725</v>
-      </c>
-      <c r="D1359" t="s">
-        <v>3726</v>
       </c>
     </row>
     <row r="1360" spans="1:4" x14ac:dyDescent="0.3">
@@ -29750,27 +29903,27 @@
         <v>2420</v>
       </c>
       <c r="B1360" t="s">
+        <v>3726</v>
+      </c>
+      <c r="C1360" t="s">
         <v>3727</v>
       </c>
-      <c r="C1360" t="s">
+      <c r="D1360" t="s">
         <v>3728</v>
-      </c>
-      <c r="D1360" t="s">
-        <v>3729</v>
       </c>
     </row>
     <row r="1361" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1361" t="s">
+        <v>3729</v>
+      </c>
+      <c r="B1361" t="s">
         <v>3730</v>
       </c>
-      <c r="B1361" t="s">
+      <c r="C1361" t="s">
         <v>3731</v>
       </c>
-      <c r="C1361" t="s">
+      <c r="D1361" t="s">
         <v>3732</v>
-      </c>
-      <c r="D1361" t="s">
-        <v>3733</v>
       </c>
     </row>
     <row r="1362" spans="1:4" x14ac:dyDescent="0.3">
@@ -29789,16 +29942,16 @@
     </row>
     <row r="1363" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1363" t="s">
+        <v>3733</v>
+      </c>
+      <c r="B1363" t="s">
         <v>3734</v>
       </c>
-      <c r="B1363" t="s">
+      <c r="C1363" t="s">
         <v>3735</v>
       </c>
-      <c r="C1363" t="s">
+      <c r="D1363" t="s">
         <v>3736</v>
-      </c>
-      <c r="D1363" t="s">
-        <v>3737</v>
       </c>
     </row>
     <row r="1365" spans="1:4" x14ac:dyDescent="0.3">
@@ -29812,7 +29965,7 @@
         <v>1452</v>
       </c>
       <c r="D1365" t="s">
-        <v>3738</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="1366" spans="1:4" x14ac:dyDescent="0.3">
@@ -29826,29 +29979,29 @@
         <v>1212</v>
       </c>
       <c r="D1366" t="s">
-        <v>3739</v>
+        <v>3738</v>
       </c>
     </row>
     <row r="1367" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1367" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B1367" t="s">
         <v>3740</v>
       </c>
-      <c r="B1367" t="s">
+      <c r="C1367" t="s">
         <v>3741</v>
       </c>
-      <c r="C1367" t="s">
+      <c r="D1367" t="s">
         <v>3742</v>
-      </c>
-      <c r="D1367" t="s">
-        <v>3743</v>
       </c>
     </row>
     <row r="1369" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1369" t="s">
+        <v>3743</v>
+      </c>
+      <c r="B1369" t="s">
         <v>3744</v>
-      </c>
-      <c r="B1369" t="s">
-        <v>3745</v>
       </c>
       <c r="C1369" t="s">
         <v>1867</v>
@@ -29859,13 +30012,13 @@
     </row>
     <row r="1370" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1370" t="s">
+        <v>3745</v>
+      </c>
+      <c r="B1370" t="s">
         <v>3746</v>
       </c>
-      <c r="B1370" t="s">
+      <c r="C1370" t="s">
         <v>3747</v>
-      </c>
-      <c r="C1370" t="s">
-        <v>3748</v>
       </c>
       <c r="D1370" t="s">
         <v>1872</v>
@@ -29873,58 +30026,58 @@
     </row>
     <row r="1371" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1371" t="s">
+        <v>3748</v>
+      </c>
+      <c r="B1371" t="s">
         <v>3749</v>
-      </c>
-      <c r="B1371" t="s">
-        <v>3750</v>
       </c>
       <c r="C1371" t="s">
         <v>2801</v>
       </c>
       <c r="D1371" t="s">
-        <v>3751</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="1372" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1372" t="s">
+        <v>3751</v>
+      </c>
+      <c r="B1372" t="s">
         <v>3752</v>
       </c>
-      <c r="B1372" t="s">
+      <c r="C1372" t="s">
         <v>3753</v>
       </c>
-      <c r="C1372" t="s">
+      <c r="D1372" t="s">
         <v>3754</v>
-      </c>
-      <c r="D1372" t="s">
-        <v>3755</v>
       </c>
     </row>
     <row r="1373" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1373" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B1373" t="s">
         <v>3756</v>
       </c>
-      <c r="B1373" t="s">
+      <c r="C1373" t="s">
         <v>3757</v>
       </c>
-      <c r="C1373" t="s">
+      <c r="D1373" t="s">
         <v>3758</v>
-      </c>
-      <c r="D1373" t="s">
-        <v>3759</v>
       </c>
     </row>
     <row r="1374" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1374" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B1374" t="s">
         <v>3760</v>
       </c>
-      <c r="B1374" t="s">
+      <c r="C1374" t="s">
         <v>3761</v>
       </c>
-      <c r="C1374" t="s">
+      <c r="D1374" t="s">
         <v>3762</v>
-      </c>
-      <c r="D1374" t="s">
-        <v>3763</v>
       </c>
     </row>
     <row r="1376" spans="1:4" x14ac:dyDescent="0.3">
@@ -29932,13 +30085,13 @@
         <v>2904</v>
       </c>
       <c r="B1376" t="s">
+        <v>3763</v>
+      </c>
+      <c r="C1376" t="s">
         <v>3764</v>
       </c>
-      <c r="C1376" t="s">
+      <c r="D1376" t="s">
         <v>3765</v>
-      </c>
-      <c r="D1376" t="s">
-        <v>3766</v>
       </c>
     </row>
     <row r="1377" spans="1:4" x14ac:dyDescent="0.3">
@@ -29946,13 +30099,13 @@
         <v>2908</v>
       </c>
       <c r="B1377" t="s">
+        <v>3766</v>
+      </c>
+      <c r="C1377" t="s">
         <v>3767</v>
       </c>
-      <c r="C1377" t="s">
+      <c r="D1377" t="s">
         <v>3768</v>
-      </c>
-      <c r="D1377" t="s">
-        <v>3769</v>
       </c>
     </row>
     <row r="1378" spans="1:4" x14ac:dyDescent="0.3">
@@ -29960,13 +30113,377 @@
         <v>2912</v>
       </c>
       <c r="B1378" t="s">
+        <v>3769</v>
+      </c>
+      <c r="C1378" t="s">
         <v>3770</v>
       </c>
-      <c r="C1378" t="s">
+      <c r="D1378" t="s">
         <v>3771</v>
       </c>
-      <c r="D1378" t="s">
+    </row>
+    <row r="1380" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1380" t="s">
         <v>3772</v>
+      </c>
+      <c r="B1380" t="s">
+        <v>3790</v>
+      </c>
+      <c r="C1380" t="s">
+        <v>3791</v>
+      </c>
+      <c r="D1380" t="s">
+        <v>3792</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1381" t="s">
+        <v>3773</v>
+      </c>
+      <c r="B1381" t="s">
+        <v>3793</v>
+      </c>
+      <c r="C1381" t="s">
+        <v>3794</v>
+      </c>
+      <c r="D1381" t="s">
+        <v>3795</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1382" t="s">
+        <v>3774</v>
+      </c>
+      <c r="B1382" t="s">
+        <v>3796</v>
+      </c>
+      <c r="C1382" t="s">
+        <v>3797</v>
+      </c>
+      <c r="D1382" t="s">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1383" t="s">
+        <v>3775</v>
+      </c>
+      <c r="B1383" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C1383" t="s">
+        <v>3800</v>
+      </c>
+      <c r="D1383" t="s">
+        <v>3801</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1384" t="s">
+        <v>3776</v>
+      </c>
+      <c r="B1384" t="s">
+        <v>3802</v>
+      </c>
+      <c r="C1384" t="s">
+        <v>3803</v>
+      </c>
+      <c r="D1384" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1386" t="s">
+        <v>3777</v>
+      </c>
+      <c r="B1386" t="s">
+        <v>3805</v>
+      </c>
+      <c r="C1386" t="s">
+        <v>3806</v>
+      </c>
+      <c r="D1386" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1387" t="s">
+        <v>2792</v>
+      </c>
+      <c r="B1387" t="s">
+        <v>3808</v>
+      </c>
+      <c r="C1387" t="s">
+        <v>3809</v>
+      </c>
+      <c r="D1387" t="s">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1388" t="s">
+        <v>2793</v>
+      </c>
+      <c r="B1388" t="s">
+        <v>3811</v>
+      </c>
+      <c r="C1388" t="s">
+        <v>3812</v>
+      </c>
+      <c r="D1388" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1389" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B1389" t="s">
+        <v>3814</v>
+      </c>
+      <c r="C1389" t="s">
+        <v>3815</v>
+      </c>
+      <c r="D1389" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1390" t="s">
+        <v>3778</v>
+      </c>
+      <c r="B1390" t="s">
+        <v>3817</v>
+      </c>
+      <c r="C1390" t="s">
+        <v>3818</v>
+      </c>
+      <c r="D1390" t="s">
+        <v>3819</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1391" t="s">
+        <v>2796</v>
+      </c>
+      <c r="B1391" t="s">
+        <v>3820</v>
+      </c>
+      <c r="C1391" t="s">
+        <v>3821</v>
+      </c>
+      <c r="D1391" t="s">
+        <v>3822</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1392" t="s">
+        <v>2797</v>
+      </c>
+      <c r="B1392" t="s">
+        <v>3823</v>
+      </c>
+      <c r="C1392" t="s">
+        <v>3824</v>
+      </c>
+      <c r="D1392" t="s">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1393" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B1393" t="s">
+        <v>3826</v>
+      </c>
+      <c r="C1393" t="s">
+        <v>3827</v>
+      </c>
+      <c r="D1393" t="s">
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1395" t="s">
+        <v>3779</v>
+      </c>
+      <c r="B1395" t="s">
+        <v>3790</v>
+      </c>
+      <c r="C1395" t="s">
+        <v>3791</v>
+      </c>
+      <c r="D1395" t="s">
+        <v>3792</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1396" t="s">
+        <v>3680</v>
+      </c>
+      <c r="B1396" t="s">
+        <v>3793</v>
+      </c>
+      <c r="C1396" t="s">
+        <v>3794</v>
+      </c>
+      <c r="D1396" t="s">
+        <v>3795</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1397" t="s">
+        <v>3780</v>
+      </c>
+      <c r="B1397" t="s">
+        <v>3796</v>
+      </c>
+      <c r="C1397" t="s">
+        <v>3797</v>
+      </c>
+      <c r="D1397" t="s">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1398" t="s">
+        <v>3682</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C1398" t="s">
+        <v>3800</v>
+      </c>
+      <c r="D1398" t="s">
+        <v>3801</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1399" t="s">
+        <v>3781</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>3802</v>
+      </c>
+      <c r="C1399" t="s">
+        <v>3803</v>
+      </c>
+      <c r="D1399" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1401" t="s">
+        <v>3782</v>
+      </c>
+      <c r="B1401" t="s">
+        <v>3805</v>
+      </c>
+      <c r="C1401" t="s">
+        <v>3806</v>
+      </c>
+      <c r="D1401" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1402" t="s">
+        <v>3783</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>3808</v>
+      </c>
+      <c r="C1402" t="s">
+        <v>3809</v>
+      </c>
+      <c r="D1402" t="s">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1403" t="s">
+        <v>3784</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>3811</v>
+      </c>
+      <c r="C1403" t="s">
+        <v>3812</v>
+      </c>
+      <c r="D1403" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1404" t="s">
+        <v>3785</v>
+      </c>
+      <c r="B1404" t="s">
+        <v>3814</v>
+      </c>
+      <c r="C1404" t="s">
+        <v>3815</v>
+      </c>
+      <c r="D1404" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1405" t="s">
+        <v>3786</v>
+      </c>
+      <c r="B1405" t="s">
+        <v>3817</v>
+      </c>
+      <c r="C1405" t="s">
+        <v>3818</v>
+      </c>
+      <c r="D1405" t="s">
+        <v>3829</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1406" t="s">
+        <v>3787</v>
+      </c>
+      <c r="B1406" t="s">
+        <v>3820</v>
+      </c>
+      <c r="C1406" t="s">
+        <v>3821</v>
+      </c>
+      <c r="D1406" t="s">
+        <v>3822</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1407" t="s">
+        <v>3788</v>
+      </c>
+      <c r="B1407" t="s">
+        <v>3823</v>
+      </c>
+      <c r="C1407" t="s">
+        <v>3824</v>
+      </c>
+      <c r="D1407" t="s">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1408" t="s">
+        <v>3789</v>
+      </c>
+      <c r="B1408" t="s">
+        <v>3826</v>
+      </c>
+      <c r="C1408" t="s">
+        <v>3827</v>
+      </c>
+      <c r="D1408" t="s">
+        <v>3828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
house language is ok
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\LandsTime-301-12-2025\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AE8146-AD86-4F82-8659-A2467E60537D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1943A019-486E-4CB6-A014-7660AD3075F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6245" uniqueCount="4520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6281" uniqueCount="4536">
   <si>
     <t>key</t>
   </si>
@@ -13616,6 +13616,54 @@
   </si>
   <si>
     <t>లోపల ఉన్నదాన్ని ఎంచుకోండి</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ లొకేషన్ నమోదు చేయండి</t>
+  </si>
+  <si>
+    <t>locality_area</t>
+  </si>
+  <si>
+    <t>Locality/Area</t>
+  </si>
+  <si>
+    <t>इलाका/क्षेत्र</t>
+  </si>
+  <si>
+    <t>ప్రాంతం/ఏరియా</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>email_address</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>ईमेल पता</t>
+  </si>
+  <si>
+    <t>ఇమెయిల్ చిరునామా</t>
+  </si>
+  <si>
+    <t>north</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>North West</t>
+  </si>
+  <si>
+    <t>उत्तर पश्चिम</t>
+  </si>
+  <si>
+    <t>South East</t>
+  </si>
+  <si>
+    <t>दक्षిణ पूर्व</t>
   </si>
 </sst>
 </file>
@@ -14002,10 +14050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D1684"/>
+  <dimension ref="A1:D1694"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1662" zoomScale="69" workbookViewId="0">
-      <selection activeCell="D1676" sqref="D1676"/>
+    <sheetView tabSelected="1" topLeftCell="A1659" zoomScale="69" workbookViewId="0">
+      <selection activeCell="A1684" sqref="A1684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36301,6 +36349,132 @@
         <v>4519</v>
       </c>
     </row>
+    <row r="1686" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1686" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B1686" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C1686" t="s">
+        <v>1484</v>
+      </c>
+      <c r="D1686" t="s">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1687" t="s">
+        <v>4521</v>
+      </c>
+      <c r="B1687" t="s">
+        <v>4522</v>
+      </c>
+      <c r="C1687" t="s">
+        <v>4523</v>
+      </c>
+      <c r="D1687" t="s">
+        <v>4524</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1688" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B1688" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C1688" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D1688" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1689" t="s">
+        <v>4525</v>
+      </c>
+      <c r="B1689" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1689" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1689" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1690" t="s">
+        <v>4526</v>
+      </c>
+      <c r="B1690" t="s">
+        <v>4527</v>
+      </c>
+      <c r="C1690" t="s">
+        <v>4528</v>
+      </c>
+      <c r="D1690" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1691" t="s">
+        <v>4530</v>
+      </c>
+      <c r="B1691" t="s">
+        <v>784</v>
+      </c>
+      <c r="C1691" t="s">
+        <v>785</v>
+      </c>
+      <c r="D1691" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1692" t="s">
+        <v>4531</v>
+      </c>
+      <c r="B1692" t="s">
+        <v>790</v>
+      </c>
+      <c r="C1692" t="s">
+        <v>791</v>
+      </c>
+      <c r="D1692" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1693" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B1693" t="s">
+        <v>4532</v>
+      </c>
+      <c r="C1693" t="s">
+        <v>4533</v>
+      </c>
+      <c r="D1693" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1694" t="s">
+        <v>2269</v>
+      </c>
+      <c r="B1694" t="s">
+        <v>4534</v>
+      </c>
+      <c r="C1694" t="s">
+        <v>4535</v>
+      </c>
+      <c r="D1694" t="s">
+        <v>799</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
search functionality is implemented 80 percent correct
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\LandsTime-301-12-2025\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1943A019-486E-4CB6-A014-7660AD3075F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33061E41-6309-484A-88F2-1D42AEA9CD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6281" uniqueCount="4536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6321" uniqueCount="4567">
   <si>
     <t>key</t>
   </si>
@@ -13664,6 +13664,99 @@
   </si>
   <si>
     <t>दक्षిణ पूर्व</t>
+  </si>
+  <si>
+    <t>search_recent</t>
+  </si>
+  <si>
+    <t>Recent Searches</t>
+  </si>
+  <si>
+    <t>ఇటీవలి శోధనలు</t>
+  </si>
+  <si>
+    <t>हाल की खोजें</t>
+  </si>
+  <si>
+    <t>search_no_results</t>
+  </si>
+  <si>
+    <t>search_try_different</t>
+  </si>
+  <si>
+    <t>Try different keywords</t>
+  </si>
+  <si>
+    <t>వేరే కీవర్డ్‌లను ప్రయత్నించండి</t>
+  </si>
+  <si>
+    <t>अलग कीवर्ड आज़माएं</t>
+  </si>
+  <si>
+    <t>search_loading</t>
+  </si>
+  <si>
+    <t>Searching...</t>
+  </si>
+  <si>
+    <t>శోధిస్తోంది...</t>
+  </si>
+  <si>
+    <t>खोज रहे हैं...</t>
+  </si>
+  <si>
+    <t>search_see_all</t>
+  </si>
+  <si>
+    <t>See All</t>
+  </si>
+  <si>
+    <t>అన్నీ చూడండి</t>
+  </si>
+  <si>
+    <t>सभी देखें</t>
+  </si>
+  <si>
+    <t>search_clear_history</t>
+  </si>
+  <si>
+    <t>Clear History</t>
+  </si>
+  <si>
+    <t>చరిత్రను క్లియర్ చేయండి</t>
+  </si>
+  <si>
+    <t>इतिहास साफ़ करें</t>
+  </si>
+  <si>
+    <t>search_results_houses</t>
+  </si>
+  <si>
+    <t>Houses</t>
+  </si>
+  <si>
+    <t>ఇళ్ళు</t>
+  </si>
+  <si>
+    <t>search_results_sites</t>
+  </si>
+  <si>
+    <t>స్థలాలు</t>
+  </si>
+  <si>
+    <t>भूमि</t>
+  </si>
+  <si>
+    <t>search_results_commercial</t>
+  </si>
+  <si>
+    <t>వాణిజ్యం</t>
+  </si>
+  <si>
+    <t>search_results_resorts</t>
+  </si>
+  <si>
+    <t>రిసార్ట్‌లు</t>
   </si>
 </sst>
 </file>
@@ -14050,10 +14143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D1694"/>
+  <dimension ref="A1:D1705"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1659" zoomScale="69" workbookViewId="0">
-      <selection activeCell="A1684" sqref="A1684"/>
+    <sheetView tabSelected="1" topLeftCell="A1677" zoomScale="69" workbookViewId="0">
+      <selection activeCell="A1708" sqref="A1708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36475,6 +36568,146 @@
         <v>799</v>
       </c>
     </row>
+    <row r="1696" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1696" t="s">
+        <v>4536</v>
+      </c>
+      <c r="B1696" t="s">
+        <v>4537</v>
+      </c>
+      <c r="C1696" t="s">
+        <v>4538</v>
+      </c>
+      <c r="D1696" t="s">
+        <v>4539</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1697" t="s">
+        <v>4540</v>
+      </c>
+      <c r="B1697" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C1697" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D1697" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1698" t="s">
+        <v>4541</v>
+      </c>
+      <c r="B1698" t="s">
+        <v>4542</v>
+      </c>
+      <c r="C1698" t="s">
+        <v>4543</v>
+      </c>
+      <c r="D1698" t="s">
+        <v>4544</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1699" t="s">
+        <v>4545</v>
+      </c>
+      <c r="B1699" t="s">
+        <v>4546</v>
+      </c>
+      <c r="C1699" t="s">
+        <v>4547</v>
+      </c>
+      <c r="D1699" t="s">
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1700" t="s">
+        <v>4549</v>
+      </c>
+      <c r="B1700" t="s">
+        <v>4550</v>
+      </c>
+      <c r="C1700" t="s">
+        <v>4551</v>
+      </c>
+      <c r="D1700" t="s">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1701" t="s">
+        <v>4553</v>
+      </c>
+      <c r="B1701" t="s">
+        <v>4554</v>
+      </c>
+      <c r="C1701" t="s">
+        <v>4555</v>
+      </c>
+      <c r="D1701" t="s">
+        <v>4556</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1702" t="s">
+        <v>4557</v>
+      </c>
+      <c r="B1702" t="s">
+        <v>4558</v>
+      </c>
+      <c r="C1702" t="s">
+        <v>4559</v>
+      </c>
+      <c r="D1702" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1703" t="s">
+        <v>4560</v>
+      </c>
+      <c r="B1703" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1703" t="s">
+        <v>4561</v>
+      </c>
+      <c r="D1703" t="s">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1704" t="s">
+        <v>4563</v>
+      </c>
+      <c r="B1704" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1704" t="s">
+        <v>4564</v>
+      </c>
+      <c r="D1704" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1705" t="s">
+        <v>4565</v>
+      </c>
+      <c r="B1705" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1705" t="s">
+        <v>4566</v>
+      </c>
+      <c r="D1705" t="s">
+        <v>1907</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edit functionality is done for the sites
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\LandsTime-301-12-2025\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33061E41-6309-484A-88F2-1D42AEA9CD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2F1D95-4804-4F39-8DF8-F384F9367B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
+    <workbookView xWindow="888" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6321" uniqueCount="4567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6353" uniqueCount="4599">
   <si>
     <t>key</t>
   </si>
@@ -13757,6 +13757,102 @@
   </si>
   <si>
     <t>రిసార్ట్‌లు</t>
+  </si>
+  <si>
+    <t>edit_property</t>
+  </si>
+  <si>
+    <t>Edit Property</t>
+  </si>
+  <si>
+    <t>प्रॉपर्टी संपादित करें</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ సవరించండి</t>
+  </si>
+  <si>
+    <t>update_property_details</t>
+  </si>
+  <si>
+    <t>Update property details</t>
+  </si>
+  <si>
+    <t>प्रॉपर्टी विवरण अपडेट करें</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ వివరాలను నవీకరించండి</t>
+  </si>
+  <si>
+    <t>updating</t>
+  </si>
+  <si>
+    <t>Updating...</t>
+  </si>
+  <si>
+    <t>अपडेट हो रहा है...</t>
+  </si>
+  <si>
+    <t>నవీకరిస్తోంది...</t>
+  </si>
+  <si>
+    <t>update_property</t>
+  </si>
+  <si>
+    <t>Update Property</t>
+  </si>
+  <si>
+    <t>प्रॉपर्टी अपडेट करें</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ నవీకరించండి</t>
+  </si>
+  <si>
+    <t>property_updated_successfully</t>
+  </si>
+  <si>
+    <t>Property updated successfully</t>
+  </si>
+  <si>
+    <t>प्रॉपर्टी सफलतापूर्वक अपडेट की गई</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ విజయవంతంగా నవీకరించబడింది</t>
+  </si>
+  <si>
+    <t>failed_to_update_property</t>
+  </si>
+  <si>
+    <t>Failed to update property</t>
+  </si>
+  <si>
+    <t>प्रॉपर्टी अपडेट करने में विफल</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ నవీకరణ విఫలమైంది</t>
+  </si>
+  <si>
+    <t>documents_locked</t>
+  </si>
+  <si>
+    <t>Documents cannot be changed during edit</t>
+  </si>
+  <si>
+    <t>संपादन के दौरान दस्तावेज़ बदले नहीं जा सकते</t>
+  </si>
+  <si>
+    <t>సవరింపు సమయంలో పత్రాలను మార్చలేరు</t>
+  </si>
+  <si>
+    <t>property_type_locked</t>
+  </si>
+  <si>
+    <t>Property type cannot be changed</t>
+  </si>
+  <si>
+    <t>प्रॉपर्टी का प्रकार बदला नहीं जा सकता</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ రకాన్ని మార్చలేరు</t>
   </si>
 </sst>
 </file>
@@ -14143,10 +14239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D1705"/>
+  <dimension ref="A1:D1713"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1677" zoomScale="69" workbookViewId="0">
-      <selection activeCell="A1708" sqref="A1708"/>
+      <selection activeCell="B1688" sqref="B1688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36708,6 +36804,118 @@
         <v>1907</v>
       </c>
     </row>
+    <row r="1706" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1706" t="s">
+        <v>4567</v>
+      </c>
+      <c r="B1706" t="s">
+        <v>4568</v>
+      </c>
+      <c r="C1706" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D1706" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1707" t="s">
+        <v>4571</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>4572</v>
+      </c>
+      <c r="C1707" t="s">
+        <v>4573</v>
+      </c>
+      <c r="D1707" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1708" t="s">
+        <v>4575</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>4576</v>
+      </c>
+      <c r="C1708" t="s">
+        <v>4577</v>
+      </c>
+      <c r="D1708" t="s">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1709" t="s">
+        <v>4579</v>
+      </c>
+      <c r="B1709" t="s">
+        <v>4580</v>
+      </c>
+      <c r="C1709" t="s">
+        <v>4581</v>
+      </c>
+      <c r="D1709" t="s">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1710" t="s">
+        <v>4583</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>4584</v>
+      </c>
+      <c r="C1710" t="s">
+        <v>4585</v>
+      </c>
+      <c r="D1710" t="s">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1711" t="s">
+        <v>4587</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>4588</v>
+      </c>
+      <c r="C1711" t="s">
+        <v>4589</v>
+      </c>
+      <c r="D1711" t="s">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1712" t="s">
+        <v>4591</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>4592</v>
+      </c>
+      <c r="C1712" t="s">
+        <v>4593</v>
+      </c>
+      <c r="D1712" t="s">
+        <v>4594</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1713" t="s">
+        <v>4595</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>4596</v>
+      </c>
+      <c r="C1713" t="s">
+        <v>4597</v>
+      </c>
+      <c r="D1713" t="s">
+        <v>4598</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
stoarge are pending for the edit
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\LandsTime-301-12-2025\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2F1D95-4804-4F39-8DF8-F384F9367B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6C7000-707F-4191-96D8-784DE6840D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14241,8 +14241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
   <dimension ref="A1:D1713"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1677" zoomScale="69" workbookViewId="0">
-      <selection activeCell="B1688" sqref="B1688"/>
+    <sheetView tabSelected="1" topLeftCell="A1696" zoomScale="69" workbookViewId="0">
+      <selection activeCell="A1714" sqref="A1714"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
my properties language translation done
</commit_message>
<xml_diff>
--- a/Frontend/translations.xlsx
+++ b/Frontend/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigat\OneDrive\Desktop\Technoji\LandsTime-301-12-2025\Landstime_Androidapp\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6C7000-707F-4191-96D8-784DE6840D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C3A809-C700-4F0A-AFA7-566BB19F89F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2932867E-4C3F-4F07-BDCC-87B15298363A}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6353" uniqueCount="4599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6497" uniqueCount="4721">
   <si>
     <t>key</t>
   </si>
@@ -13853,6 +13853,372 @@
   </si>
   <si>
     <t>ప్రాపర్టీ రకాన్ని మార్చలేరు</t>
+  </si>
+  <si>
+    <t>my_properties_title</t>
+  </si>
+  <si>
+    <t>నా ప్రాపర్టీలు</t>
+  </si>
+  <si>
+    <t>मेरी संपत्तियां</t>
+  </si>
+  <si>
+    <t>my_properties_search_placeholder</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీలు వెతకండి...</t>
+  </si>
+  <si>
+    <t>संपत्तियां खोजें...</t>
+  </si>
+  <si>
+    <t>tab_all</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>అన్నీ</t>
+  </si>
+  <si>
+    <t>सभी</t>
+  </si>
+  <si>
+    <t>tab_active</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>యాక్టివ్</t>
+  </si>
+  <si>
+    <t>सक्रिय</t>
+  </si>
+  <si>
+    <t>tab_pending</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>పెండింగ్</t>
+  </si>
+  <si>
+    <t>लंबित</t>
+  </si>
+  <si>
+    <t>tab_sold</t>
+  </si>
+  <si>
+    <t>Sold</t>
+  </si>
+  <si>
+    <t>అమ్మబడింది</t>
+  </si>
+  <si>
+    <t>बेचा गया</t>
+  </si>
+  <si>
+    <t>status_active</t>
+  </si>
+  <si>
+    <t>status_pending_review</t>
+  </si>
+  <si>
+    <t>Pending Review</t>
+  </si>
+  <si>
+    <t>సమీక్ష పెండింగ్</t>
+  </si>
+  <si>
+    <t>समीक्षा लंबित</t>
+  </si>
+  <si>
+    <t>status_rejected</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>తిరస్కరించబడింది</t>
+  </si>
+  <si>
+    <t>अस्वीकृत</t>
+  </si>
+  <si>
+    <t>status_sold_out</t>
+  </si>
+  <si>
+    <t>Sold Out</t>
+  </si>
+  <si>
+    <t>बिक गया</t>
+  </si>
+  <si>
+    <t>edit_to_resubmit</t>
+  </si>
+  <si>
+    <t>Edit to resubmit</t>
+  </si>
+  <si>
+    <t>మళ్ళీ సమర్పించడానికి సవరించండి</t>
+  </si>
+  <si>
+    <t>पुनः सबमिट करने के लिए संपादित करें</t>
+  </si>
+  <si>
+    <t>no_reviews_yet</t>
+  </si>
+  <si>
+    <t>No reviews yet</t>
+  </si>
+  <si>
+    <t>ఇంకా సమీక్షలు లేవు</t>
+  </si>
+  <si>
+    <t>अभी कोई समीक्षा नहीं</t>
+  </si>
+  <si>
+    <t>loading_properties</t>
+  </si>
+  <si>
+    <t>Loading properties...</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీలు లోడ్ అవుతున్నాయి...</t>
+  </si>
+  <si>
+    <t>संपत्तियां लोड हो रही हैं...</t>
+  </si>
+  <si>
+    <t>no_properties_found</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీలు కనుగొనబడలేదు</t>
+  </si>
+  <si>
+    <t>no_properties_added</t>
+  </si>
+  <si>
+    <t>You haven't added any properties yet</t>
+  </si>
+  <si>
+    <t>మీరు ఇంకా ఏ ప్రాపర్టీలు జోడించలేదు</t>
+  </si>
+  <si>
+    <t>आपने अभी तक कोई संपत्ति नहीं जोड़ी</t>
+  </si>
+  <si>
+    <t>no_properties_in_tab</t>
+  </si>
+  <si>
+    <t>No {tab} properties</t>
+  </si>
+  <si>
+    <t>{tab} ప్రాపర్టీలు లేవు</t>
+  </si>
+  <si>
+    <t>कोई {tab} संपत्ति नहीं</t>
+  </si>
+  <si>
+    <t>search_no_match</t>
+  </si>
+  <si>
+    <t>No properties match "{query}"</t>
+  </si>
+  <si>
+    <t>{query} కు సరిపోలే ప్రాపర్టీలు లేవు</t>
+  </si>
+  <si>
+    <t>{query} से मेल खाती कोई संपत्ति नहीं</t>
+  </si>
+  <si>
+    <t>untitled_property</t>
+  </si>
+  <si>
+    <t>Untitled Property</t>
+  </si>
+  <si>
+    <t>శీర్షిక లేని ప్రాపర్టీ</t>
+  </si>
+  <si>
+    <t>बिना शीर्षक की संपत्ति</t>
+  </si>
+  <si>
+    <t>location_not_specified</t>
+  </si>
+  <si>
+    <t>Location not specified</t>
+  </si>
+  <si>
+    <t>స్థానం పేర్కొనబడలేదు</t>
+  </si>
+  <si>
+    <t>स्थान निर्दिष्ट नहीं</t>
+  </si>
+  <si>
+    <t>btn_view</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>చూడండి</t>
+  </si>
+  <si>
+    <t>देखें</t>
+  </si>
+  <si>
+    <t>options_title</t>
+  </si>
+  <si>
+    <t>Property Options</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ ఎంపికలు</t>
+  </si>
+  <si>
+    <t>संपत्ति विकल्प</t>
+  </si>
+  <si>
+    <t>option_edit</t>
+  </si>
+  <si>
+    <t>संपत्ति संपादित करें</t>
+  </si>
+  <si>
+    <t>option_cannot_edit_sold</t>
+  </si>
+  <si>
+    <t>Cannot Edit (Sold)</t>
+  </si>
+  <si>
+    <t>సవరించలేరు (అమ్మబడింది)</t>
+  </si>
+  <si>
+    <t>संपादित नहीं कर सकते (बेचा गया)</t>
+  </si>
+  <si>
+    <t>option_resubmit_note</t>
+  </si>
+  <si>
+    <t>Property will be resubmitted for review</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ సమీక్షకు మళ్ళీ సమర్పించబడుతుంది</t>
+  </si>
+  <si>
+    <t>संपत्ति समीक्षा के लिए पुनः सबमिट की जाएगी</t>
+  </si>
+  <si>
+    <t>option_mark_sold</t>
+  </si>
+  <si>
+    <t>Mark as Sold</t>
+  </si>
+  <si>
+    <t>అమ్మినట్లు గుర్తించండి</t>
+  </si>
+  <si>
+    <t>बेचा गया चिह्नित करें</t>
+  </si>
+  <si>
+    <t>option_already_sold</t>
+  </si>
+  <si>
+    <t>Already Sold</t>
+  </si>
+  <si>
+    <t>ఇప్పటికే అమ్మబడింది</t>
+  </si>
+  <si>
+    <t>पहले से बेचा गया</t>
+  </si>
+  <si>
+    <t>btn_cancel</t>
+  </si>
+  <si>
+    <t>రద్దు చేయి</t>
+  </si>
+  <si>
+    <t>mark_sold_title</t>
+  </si>
+  <si>
+    <t>mark_sold_message</t>
+  </si>
+  <si>
+    <t>Are you sure you want to mark this property as sold? This action cannot be undone by you.</t>
+  </si>
+  <si>
+    <t>మీరు ఈ ప్రాపర్టీని అమ్మినట్లు గుర్తించాలనుకుంటున్నారా? ఈ చర్యను మీరు రద్దు చేయలేరు.</t>
+  </si>
+  <si>
+    <t>क्या आप वाकई इस संपत्ति को बेचा गया चिह्नित करना चाहते हैं? यह क्रिया आप पूर्ववत नहीं कर सकते।</t>
+  </si>
+  <si>
+    <t>mark_sold_confirm</t>
+  </si>
+  <si>
+    <t>success_marked_sold</t>
+  </si>
+  <si>
+    <t>Property marked as sold</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీ అమ్మినట్లు గుర్తించబడింది</t>
+  </si>
+  <si>
+    <t>संपत्ति बेचा गया चिह्नित की गई</t>
+  </si>
+  <si>
+    <t>error_mark_sold</t>
+  </si>
+  <si>
+    <t>Failed to mark property as sold</t>
+  </si>
+  <si>
+    <t>ప్రాపర్టీని అమ్మినట్లు గుర్తించడం విఫలమైంది</t>
+  </si>
+  <si>
+    <t>संपत्ति को बेचा गया चिह्नित करना विफल रहा</t>
+  </si>
+  <si>
+    <t>voice_search_not_supported</t>
+  </si>
+  <si>
+    <t>Voice search is not supported in this browser</t>
+  </si>
+  <si>
+    <t>ఈ బ్రౌజర్‌లో వాయిస్ సెర్చ్ మద్దతు లేదు</t>
+  </si>
+  <si>
+    <t>इस ब्राउज़र में वॉइस सर्च समर्थित नहीं है</t>
+  </si>
+  <si>
+    <t>review_singular</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>సమీక్ష</t>
+  </si>
+  <si>
+    <t>समीक्षा</t>
+  </si>
+  <si>
+    <t>review_plural</t>
+  </si>
+  <si>
+    <t>reviews</t>
+  </si>
+  <si>
+    <t>సమీక్షలు</t>
+  </si>
+  <si>
+    <t>समीक्षाएं</t>
   </si>
 </sst>
 </file>
@@ -14239,10 +14605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4B5E5-1AD3-459E-940E-0D51EC173CF5}">
-  <dimension ref="A1:D1713"/>
+  <dimension ref="A1:D1750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1696" zoomScale="69" workbookViewId="0">
-      <selection activeCell="A1714" sqref="A1714"/>
+    <sheetView tabSelected="1" topLeftCell="A1691" zoomScale="69" workbookViewId="0">
+      <selection activeCell="A1715" sqref="A1715"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36916,6 +37282,510 @@
         <v>4598</v>
       </c>
     </row>
+    <row r="1715" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1715" t="s">
+        <v>4599</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C1715" t="s">
+        <v>4601</v>
+      </c>
+      <c r="D1715" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1716" t="s">
+        <v>4602</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>4604</v>
+      </c>
+      <c r="D1716" t="s">
+        <v>4603</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1717" t="s">
+        <v>4605</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>4606</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>4608</v>
+      </c>
+      <c r="D1717" t="s">
+        <v>4607</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1718" t="s">
+        <v>4609</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>4610</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>4612</v>
+      </c>
+      <c r="D1718" t="s">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1719" t="s">
+        <v>4613</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>4614</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>4616</v>
+      </c>
+      <c r="D1719" t="s">
+        <v>4615</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1720" t="s">
+        <v>4617</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>4618</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>4620</v>
+      </c>
+      <c r="D1720" t="s">
+        <v>4619</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1721" t="s">
+        <v>4621</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>4610</v>
+      </c>
+      <c r="C1721" t="s">
+        <v>4612</v>
+      </c>
+      <c r="D1721" t="s">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1722" t="s">
+        <v>4622</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>4623</v>
+      </c>
+      <c r="C1722" t="s">
+        <v>4625</v>
+      </c>
+      <c r="D1722" t="s">
+        <v>4624</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1723" t="s">
+        <v>4626</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>4627</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>4629</v>
+      </c>
+      <c r="D1723" t="s">
+        <v>4628</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1724" t="s">
+        <v>4630</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>4631</v>
+      </c>
+      <c r="C1724" t="s">
+        <v>4632</v>
+      </c>
+      <c r="D1724" t="s">
+        <v>4619</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1725" t="s">
+        <v>4633</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>4634</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>4636</v>
+      </c>
+      <c r="D1725" t="s">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1726" t="s">
+        <v>4637</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>4638</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>4640</v>
+      </c>
+      <c r="D1726" t="s">
+        <v>4639</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1727" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1727" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1728" t="s">
+        <v>4641</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>4642</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>4644</v>
+      </c>
+      <c r="D1728" t="s">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1729" t="s">
+        <v>4645</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D1729" t="s">
+        <v>4646</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1730" t="s">
+        <v>4647</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>4648</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>4650</v>
+      </c>
+      <c r="D1730" t="s">
+        <v>4649</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1731" t="s">
+        <v>4651</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>4652</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>4654</v>
+      </c>
+      <c r="D1731" t="s">
+        <v>4653</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1732" t="s">
+        <v>4655</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>4656</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>4658</v>
+      </c>
+      <c r="D1732" t="s">
+        <v>4657</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1733" t="s">
+        <v>4659</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>4660</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>4662</v>
+      </c>
+      <c r="D1733" t="s">
+        <v>4661</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1734" t="s">
+        <v>4663</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>4664</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>4666</v>
+      </c>
+      <c r="D1734" t="s">
+        <v>4665</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1735" t="s">
+        <v>4667</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>4668</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>4670</v>
+      </c>
+      <c r="D1735" t="s">
+        <v>4669</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1736" t="s">
+        <v>4671</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>4672</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>4674</v>
+      </c>
+      <c r="D1736" t="s">
+        <v>4673</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1737" t="s">
+        <v>4675</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>4568</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>4676</v>
+      </c>
+      <c r="D1737" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1738" t="s">
+        <v>4677</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>4678</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>4680</v>
+      </c>
+      <c r="D1738" t="s">
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1739" t="s">
+        <v>4681</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>4682</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>4684</v>
+      </c>
+      <c r="D1739" t="s">
+        <v>4683</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1740" t="s">
+        <v>4685</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>4686</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>4688</v>
+      </c>
+      <c r="D1740" t="s">
+        <v>4687</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1741" t="s">
+        <v>4689</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>4690</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>4692</v>
+      </c>
+      <c r="D1741" t="s">
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1742" t="s">
+        <v>4693</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D1742" t="s">
+        <v>4694</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1743" t="s">
+        <v>4695</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>4686</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>4688</v>
+      </c>
+      <c r="D1743" t="s">
+        <v>4687</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1744" t="s">
+        <v>4696</v>
+      </c>
+      <c r="B1744" t="s">
+        <v>4697</v>
+      </c>
+      <c r="C1744" t="s">
+        <v>4699</v>
+      </c>
+      <c r="D1744" t="s">
+        <v>4698</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1745" t="s">
+        <v>4700</v>
+      </c>
+      <c r="B1745" t="s">
+        <v>4686</v>
+      </c>
+      <c r="C1745" t="s">
+        <v>4688</v>
+      </c>
+      <c r="D1745" t="s">
+        <v>4687</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1746" t="s">
+        <v>4701</v>
+      </c>
+      <c r="B1746" t="s">
+        <v>4702</v>
+      </c>
+      <c r="C1746" t="s">
+        <v>4704</v>
+      </c>
+      <c r="D1746" t="s">
+        <v>4703</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1747" t="s">
+        <v>4705</v>
+      </c>
+      <c r="B1747" t="s">
+        <v>4706</v>
+      </c>
+      <c r="C1747" t="s">
+        <v>4708</v>
+      </c>
+      <c r="D1747" t="s">
+        <v>4707</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1748" t="s">
+        <v>4709</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>4710</v>
+      </c>
+      <c r="C1748" t="s">
+        <v>4712</v>
+      </c>
+      <c r="D1748" t="s">
+        <v>4711</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1749" t="s">
+        <v>4713</v>
+      </c>
+      <c r="B1749" t="s">
+        <v>4714</v>
+      </c>
+      <c r="C1749" t="s">
+        <v>4716</v>
+      </c>
+      <c r="D1749" t="s">
+        <v>4715</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1750" t="s">
+        <v>4717</v>
+      </c>
+      <c r="B1750" t="s">
+        <v>4718</v>
+      </c>
+      <c r="C1750" t="s">
+        <v>4720</v>
+      </c>
+      <c r="D1750" t="s">
+        <v>4719</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>